<commit_message>
Added new store mount
</commit_message>
<xml_diff>
--- a/Lib/Mounts.xlsx
+++ b/Lib/Mounts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3954" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3957" uniqueCount="762">
   <si>
     <t>Invincible's Reins</t>
   </si>
@@ -2299,6 +2299,12 @@
   </si>
   <si>
     <t>Send to Addon</t>
+  </si>
+  <si>
+    <t>Kalu'ak Whalebone Glider</t>
+  </si>
+  <si>
+    <t>Glider</t>
   </si>
 </sst>
 </file>
@@ -2352,16 +2358,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2393,7 +2392,34 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -2427,7 +2453,7 @@
     <tableColumn id="4" name="Faction"/>
     <tableColumn id="5" name="SpellID"/>
     <tableColumn id="6" name="Speed"/>
-    <tableColumn id="7" name="link" dataDxfId="9">
+    <tableColumn id="7" name="link" dataDxfId="11">
       <calculatedColumnFormula>CONCATENATE("https://www.wowhead.com/wotlk/item=",A2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2445,16 +2471,16 @@
     <tableColumn id="1" name="Spell ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Category"/>
-    <tableColumn id="4" name="Speed" dataDxfId="8"/>
-    <tableColumn id="5" name="ItemID" dataDxfId="7"/>
+    <tableColumn id="4" name="Speed" dataDxfId="10"/>
+    <tableColumn id="5" name="ItemID" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:O370" totalsRowShown="0">
-  <autoFilter ref="A1:O370">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:O371" totalsRowShown="0">
+  <autoFilter ref="A1:O371">
     <filterColumn colId="11">
       <filters>
         <filter val="1"/>
@@ -2469,7 +2495,7 @@
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Category"/>
     <tableColumn id="4" name="Speed"/>
-    <tableColumn id="11" name="MinSpeed" dataDxfId="6"/>
+    <tableColumn id="11" name="MinSpeed" dataDxfId="5"/>
     <tableColumn id="12" name="SwimSpeed"/>
     <tableColumn id="5" name="ItemID"/>
     <tableColumn id="8" name="Source"/>
@@ -2480,10 +2506,10 @@
     <tableColumn id="14" name="MountKey" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE(Table3[[#This Row],[Spell ID]]," - ",Table3[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table Data" dataDxfId="3">
-      <calculatedColumnFormula>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</calculatedColumnFormula>
+    <tableColumn id="6" name="Table Data" dataDxfId="0">
+      <calculatedColumnFormula>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Link" dataDxfId="5">
+    <tableColumn id="7" name="Link" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22797,11 +22823,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O370"/>
+  <dimension ref="A1:O371"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N318" sqref="N318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22817,7 +22843,8 @@
     <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.36328125" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="42.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22904,8 +22931,8 @@
         <v>0 - 875</v>
       </c>
       <c r="N2" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 875"] +{"Brown Horse", 0, 875, 0.6, 0.6, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 875"] ={"Brown Horse", 0, 875, 0.6, 0.6, 0, "Horse", "removed"},</v>
       </c>
       <c r="O2" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -22948,8 +22975,8 @@
         <v>0 - 8589</v>
       </c>
       <c r="N3" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 8589"] +{"Ivory Raptor", 0, 8589, 0.6, 0.6, 0, "Raptor", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 8589"] ={"Ivory Raptor", 0, 8589, 0.6, 0.6, 0, "Raptor", "removed"},</v>
       </c>
       <c r="O3" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -22992,8 +23019,8 @@
         <v>0 - 8627</v>
       </c>
       <c r="N4" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 8627"] +{"Nightsaber", 0, 8627, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 8627"] ={"Nightsaber", 0, 8627, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O4" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23036,8 +23063,8 @@
         <v>0 - 8628</v>
       </c>
       <c r="N5" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 8628"] +{"Spotted Nightsaber", 0, 8628, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 8628"] ={"Spotted Nightsaber", 0, 8628, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O5" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23080,8 +23107,8 @@
         <v>0 - 8630</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 8630"] +{"Bengal Tiger", 0, 8630, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 8630"] ={"Bengal Tiger", 0, 8630, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O6" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23124,8 +23151,8 @@
         <v>0 - 8633</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 8633"] +{"Leopard", 0, 8633, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 8633"] ={"Leopard", 0, 8633, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O7" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23168,8 +23195,8 @@
         <v>0 - 12351</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 12351"] +{"Arctic Wolf", 0, 12351, 1, 1, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 12351"] ={"Arctic Wolf", 0, 12351, 1, 1, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O8" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23212,8 +23239,8 @@
         <v>0 - 13332</v>
       </c>
       <c r="N9" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 13332"] +{"Blue Skeletal Horse", 0, 13332, 0.6, 0.6, 0, "Horse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 13332"] ={"Blue Skeletal Horse", 0, 13332, 0.6, 0.6, 0, "Horse", "Gold"},</v>
       </c>
       <c r="O9" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23256,8 +23283,8 @@
         <v>0 - 16338</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 16338"] +{"Knight-Lieutenant's Steed", 0, 16338, 0.6, 0.6, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 16338"] ={"Knight-Lieutenant's Steed", 0, 16338, 0.6, 0.6, 0, "Horse", "removed"},</v>
       </c>
       <c r="O10" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23297,8 +23324,8 @@
         <v>0 - 16339</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 16339"] +{"Commander's Steed", 0, 16339, 1, 1, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 16339"] ={"Commander's Steed", 0, 16339, 1, 1, 0, "Horse", "removed"},</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23341,8 +23368,8 @@
         <v>0 - 16343</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 16343"] +{"Blood Guard's Mount", 0, 16343, 0.6, 0.6, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 16343"] ={"Blood Guard's Mount", 0, 16343, 0.6, 0.6, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23385,8 +23412,8 @@
         <v>0 - 16344</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 16344"] +{"zzUNUSEDLieutenant General's Mount", 0, 16344, 0.6, 0.6, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 16344"] ={"zzUNUSEDLieutenant General's Mount", 0, 16344, 0.6, 0.6, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23432,8 +23459,8 @@
         <v>0 - 20221</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 20221"] +{"Fabled Steed", 0, 20221, 1, 1, 0, "Drake", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 20221"] ={"Fabled Steed", 0, 20221, 1, 1, 0, "Drake", "removed"},</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23476,8 +23503,8 @@
         <v>0 - 27819</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 27819"] +{"Crazy Raptor 75", 0, 27819, 1, 1, 0, "Raptor", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 27819"] ={"Crazy Raptor 75", 0, 27819, 1, 1, 0, "Raptor", "removed"},</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23520,8 +23547,8 @@
         <v>0 - 27853</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 27853"] +{"Crazy Raptor 150", 0, 27853, 1, 1, 0, "Raptor", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 27853"] ={"Crazy Raptor 150", 0, 27853, 1, 1, 0, "Raptor", "removed"},</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23564,8 +23591,8 @@
         <v>0 - 28289</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 28289"] +{"Dargonhawk Whistle", 0, 28289, 0.6, 0.6, 0, "Unknown", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 28289"] ={"Dargonhawk Whistle", 0, 28289, 0.6, 0.6, 0, "Unknown", "removed"},</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23608,8 +23635,8 @@
         <v>0 - 29225</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 29225"] +{"zzoldSwift Warstrider", 0, 29225, 1, 1, 0, "Hawkstrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 29225"] ={"zzoldSwift Warstrider", 0, 29225, 1, 1, 0, "Hawkstrider", "removed"},</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23655,8 +23682,8 @@
         <v>0 - 38265</v>
       </c>
       <c r="N19" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 38265"] +{"Black Warp Stalker", 0, 38265, 1, 1, 0, "Warp Stalker", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 38265"] ={"Black Warp Stalker", 0, 38265, 1, 1, 0, "Warp Stalker", "removed"},</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23699,8 +23726,8 @@
         <v>0 - 44229</v>
       </c>
       <c r="N20" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 44229"] +{"Loaned Wind Rider Reins", 0, 44229, 1.5, 1.5, 0, "Wind Rider", "Quest"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 44229"] ={"Loaned Wind Rider Reins", 0, 44229, 1.5, 1.5, 0, "Wind Rider", "Quest"},</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23746,8 +23773,8 @@
         <v>0 - 49289</v>
       </c>
       <c r="N21" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["0 - 49289"] +{"Little White Stallion", 0, 49289, 0.6, 0.6, 0, "Horse", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["0 - 49289"] ={"Little White Stallion", 0, 49289, 0.6, 0.6, 0, "Horse", "Removed"},</v>
       </c>
       <c r="O21" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23793,8 +23820,8 @@
         <v>458 - 5656</v>
       </c>
       <c r="N22" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["458 - 5656"] +{"Brown Horse", 458, 5656, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["458 - 5656"] ={"Brown Horse", 458, 5656, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O22" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23837,8 +23864,8 @@
         <v>459 - 1134</v>
       </c>
       <c r="N23" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["459 - 1134"] +{"Gray Wolf", 459, 1134, 0.6, 0.6, 0, "Wolf", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["459 - 1134"] ={"Gray Wolf", 459, 1134, 0.6, 0.6, 0, "Wolf", "Removed"},</v>
       </c>
       <c r="O23" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23881,8 +23908,8 @@
         <v>468 - 2415</v>
       </c>
       <c r="N24" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["468 - 2415"] +{"White Stallion", 468, 2415, 0.6, 0.6, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["468 - 2415"] ={"White Stallion", 468, 2415, 0.6, 0.6, 0, "Horse", "removed"},</v>
       </c>
       <c r="O24" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23928,8 +23955,8 @@
         <v>470 - 2411</v>
       </c>
       <c r="N25" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["470 - 2411"] +{"Black Stallion", 470, 2411, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["470 - 2411"] ={"Black Stallion", 470, 2411, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O25" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -23972,8 +23999,8 @@
         <v>471 - 2413</v>
       </c>
       <c r="N26" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["471 - 2413"] +{"Palamino", 471, 2413, 0.6, 0.6, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["471 - 2413"] ={"Palamino", 471, 2413, 0.6, 0.6, 0, "Horse", "removed"},</v>
       </c>
       <c r="O26" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24019,8 +24046,8 @@
         <v>472 - 2414</v>
       </c>
       <c r="N27" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["472 - 2414"] +{"Pinto", 472, 2414, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["472 - 2414"] ={"Pinto", 472, 2414, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O27" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24063,8 +24090,8 @@
         <v>578 - 1041</v>
       </c>
       <c r="N28" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["578 - 1041"] +{"Black Wolf", 578, 1041, 0.6, 0.6, 0, "Wolf", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["578 - 1041"] ={"Black Wolf", 578, 1041, 0.6, 0.6, 0, "Wolf", "Removed"},</v>
       </c>
       <c r="O28" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24107,8 +24134,8 @@
         <v>579 - 5663</v>
       </c>
       <c r="N29" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["579 - 5663"] +{"Red Wolf", 579, 5663, 1, 1, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["579 - 5663"] ={"Red Wolf", 579, 5663, 1, 1, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O29" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24151,8 +24178,8 @@
         <v>580 - 1132</v>
       </c>
       <c r="N30" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["580 - 1132"] +{"Timber Wolf", 580, 1132, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["580 - 1132"] ={"Timber Wolf", 580, 1132, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O30" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24195,8 +24222,8 @@
         <v>581 - 1133</v>
       </c>
       <c r="N31" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["581 - 1133"] +{"Winter Wolf", 581, 1133, 0.6, 0.6, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["581 - 1133"] ={"Winter Wolf", 581, 1133, 0.6, 0.6, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O31" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24242,8 +24269,8 @@
         <v>3363 - 21736</v>
       </c>
       <c r="N32" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["3363 - 21736"] +{"Nether Drake", 3363, 21736, 3.1, 3.1, 0, "Nether Drake", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["3363 - 21736"] ={"Nether Drake", 3363, 21736, 3.1, 3.1, 0, "Nether Drake", "removed"},</v>
       </c>
       <c r="O32" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24289,8 +24316,8 @@
         <v>5784 - 0</v>
       </c>
       <c r="N33" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["5784 - 0"] +{"Felsteed", 5784, 0, 0.6, 0.6, 0, "Warlock", "Warlock"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["5784 - 0"] ={"Felsteed", 5784, 0, 0.6, 0.6, 0, "Warlock", "Warlock"},</v>
       </c>
       <c r="O33" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24336,8 +24363,8 @@
         <v>6648 - 5655</v>
       </c>
       <c r="N34" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6648 - 5655"] +{"Chestnut Mare", 6648, 5655, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6648 - 5655"] ={"Chestnut Mare", 6648, 5655, 0.6, 0.6, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O34" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24380,8 +24407,8 @@
         <v>6653 - 5665</v>
       </c>
       <c r="N35" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6653 - 5665"] +{"Dire Wolf", 6653, 5665, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6653 - 5665"] ={"Dire Wolf", 6653, 5665, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O35" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24424,8 +24451,8 @@
         <v>6654 - 5668</v>
       </c>
       <c r="N36" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6654 - 5668"] +{"Brown Wolf", 6654, 5668, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6654 - 5668"] ={"Brown Wolf", 6654, 5668, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O36" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24471,8 +24498,8 @@
         <v>6777 - 5864</v>
       </c>
       <c r="N37" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6777 - 5864"] +{"Gray Ram", 6777, 5864, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6777 - 5864"] ={"Gray Ram", 6777, 5864, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O37" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24515,8 +24542,8 @@
         <v>6896 - 5874</v>
       </c>
       <c r="N38" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6896 - 5874"] +{"Black Ram", 6896, 5874, 0.6, 0.6, 0, "Ram", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6896 - 5874"] ={"Black Ram", 6896, 5874, 0.6, 0.6, 0, "Ram", "Removed"},</v>
       </c>
       <c r="O38" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24559,8 +24586,8 @@
         <v>6897 - 5875</v>
       </c>
       <c r="N39" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6897 - 5875"] +{"Blue Ram", 6897, 5875, 0.6, 0.6, 0, "Ram", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6897 - 5875"] ={"Blue Ram", 6897, 5875, 0.6, 0.6, 0, "Ram", "Removed"},</v>
       </c>
       <c r="O39" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24606,8 +24633,8 @@
         <v>6898 - 5873</v>
       </c>
       <c r="N40" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6898 - 5873"] +{"White Ram", 6898, 5873, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6898 - 5873"] ={"White Ram", 6898, 5873, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O40" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24653,8 +24680,8 @@
         <v>6899 - 5872</v>
       </c>
       <c r="N41" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["6899 - 5872"] +{"Brown Ram", 6899, 5872, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["6899 - 5872"] ={"Brown Ram", 6899, 5872, 0.6, 0.6, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O41" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24700,8 +24727,8 @@
         <v>8394 - 8631</v>
       </c>
       <c r="N42" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["8394 - 8631"] +{"Striped Frostsaber", 8394, 8631, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["8394 - 8631"] ={"Striped Frostsaber", 8394, 8631, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O42" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24744,8 +24771,8 @@
         <v>8395 - 8588</v>
       </c>
       <c r="N43" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["8395 - 8588"] +{"Emerald Raptor", 8395, 8588, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["8395 - 8588"] ={"Emerald Raptor", 8395, 8588, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O43" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24788,8 +24815,8 @@
         <v>8595 - 28025</v>
       </c>
       <c r="N44" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["8595 - 28025"] +{"Blue Mechanostrider", 8595, 28025, 1, 1, 0, "Mechanostrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["8595 - 28025"] ={"Blue Mechanostrider", 8595, 28025, 1, 1, 0, "Mechanostrider", "removed"},</v>
       </c>
       <c r="O44" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24832,8 +24859,8 @@
         <v>8980 - 8583</v>
       </c>
       <c r="N45" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["8980 - 8583"] +{"Skeletal Horse", 8980, 8583, 0.6, 0.6, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["8980 - 8583"] ={"Skeletal Horse", 8980, 8583, 0.6, 0.6, 0, "Horse", "removed"},</v>
       </c>
       <c r="O45" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24879,8 +24906,8 @@
         <v>10789 - 8632</v>
       </c>
       <c r="N46" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10789 - 8632"] +{"Spotted Frostsaber", 10789, 8632, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10789 - 8632"] ={"Spotted Frostsaber", 10789, 8632, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O46" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24926,8 +24953,8 @@
         <v>10793 - 8629</v>
       </c>
       <c r="N47" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10793 - 8629"] +{"Striped Nightsaber", 10793, 8629, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10793 - 8629"] ={"Striped Nightsaber", 10793, 8629, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O47" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -24973,8 +25000,8 @@
         <v>10795 - 49288</v>
       </c>
       <c r="N48" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10795 - 49288"] +{"Ivory Raptor", 10795, 49288, 0.6, 0.6, 0, "Raptor", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10795 - 49288"] ={"Ivory Raptor", 10795, 49288, 0.6, 0.6, 0, "Raptor", "TCG"},</v>
       </c>
       <c r="O48" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25017,8 +25044,8 @@
         <v>10796 - 8591</v>
       </c>
       <c r="N49" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10796 - 8591"] +{"Turquoise Raptor", 10796, 8591, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10796 - 8591"] ={"Turquoise Raptor", 10796, 8591, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O49" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25061,8 +25088,8 @@
         <v>10798 - 8590</v>
       </c>
       <c r="N50" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10798 - 8590"] +{"Obsidian Raptor", 10798, 8590, 0.6, 0.6, 0, "Raptor", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10798 - 8590"] ={"Obsidian Raptor", 10798, 8590, 0.6, 0.6, 0, "Raptor", "removed"},</v>
       </c>
       <c r="O50" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25105,8 +25132,8 @@
         <v>10799 - 8592</v>
       </c>
       <c r="N51" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10799 - 8592"] +{"Violet Raptor", 10799, 8592, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10799 - 8592"] ={"Violet Raptor", 10799, 8592, 0.6, 0.6, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O51" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25152,8 +25179,8 @@
         <v>10873 - 8563</v>
       </c>
       <c r="N52" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10873 - 8563"] +{"Red Mechanostrider", 10873, 8563, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10873 - 8563"] ={"Red Mechanostrider", 10873, 8563, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O52" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25196,8 +25223,8 @@
         <v>10969 - 8595</v>
       </c>
       <c r="N53" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["10969 - 8595"] +{"Blue Mechanostrider", 10969, 8595, 0.6, 0.6, 0, "Mechanostrider", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["10969 - 8595"] ={"Blue Mechanostrider", 10969, 8595, 0.6, 0.6, 0, "Mechanostrider", "Duplicate"},</v>
       </c>
       <c r="O53" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25243,8 +25270,8 @@
         <v>13819 - 0</v>
       </c>
       <c r="N54" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["13819 - 0"] +{"Warhorse", 13819, 0, 0.6, 0.6, 0, "Paladin", "Paladin"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["13819 - 0"] ={"Warhorse", 13819, 0, 0.6, 0.6, 0, "Paladin", "Paladin"},</v>
       </c>
       <c r="O54" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25287,8 +25314,8 @@
         <v>15779 - 13326</v>
       </c>
       <c r="N55" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["15779 - 13326"] +{"White Mechanostrider Mod B", 15779, 13326, 1, 1, 0, "Mechanostrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["15779 - 13326"] ={"White Mechanostrider Mod B", 15779, 13326, 1, 1, 0, "Mechanostrider", "removed"},</v>
       </c>
       <c r="O55" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25331,8 +25358,8 @@
         <v>15780 - 13321</v>
       </c>
       <c r="N56" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["15780 - 13321"] +{"Green Mechanostrider", 15780, 13321, 0.6, 0.6, 0, "Mechanostrider", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["15780 - 13321"] ={"Green Mechanostrider", 15780, 13321, 0.6, 0.6, 0, "Mechanostrider", "Removed"},</v>
       </c>
       <c r="O56" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25375,8 +25402,8 @@
         <v>15787 - 0</v>
       </c>
       <c r="N57" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["15787 - 0"] +{"Steel Mechanostrider", 15787, 0, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["15787 - 0"] ={"Steel Mechanostrider", 15787, 0, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
       </c>
       <c r="O57" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25419,8 +25446,8 @@
         <v>16055 - 12303</v>
       </c>
       <c r="N58" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16055 - 12303"] +{"Black Nightsaber", 16055, 12303, 1, 1, 0, "Saber", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16055 - 12303"] ={"Black Nightsaber", 16055, 12303, 1, 1, 0, "Saber", "Removed"},</v>
       </c>
       <c r="O58" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25463,8 +25490,8 @@
         <v>16056 - 12302</v>
       </c>
       <c r="N59" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16056 - 12302"] +{"Ancient Frostsaber", 16056, 12302, 1, 1, 0, "Saber", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16056 - 12302"] ={"Ancient Frostsaber", 16056, 12302, 1, 1, 0, "Saber", "Removed"},</v>
       </c>
       <c r="O59" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25507,8 +25534,8 @@
         <v>16058 - 12325</v>
       </c>
       <c r="N60" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16058 - 12325"] +{"Primal Leopard", 16058, 12325, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16058 - 12325"] ={"Primal Leopard", 16058, 12325, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O60" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25551,8 +25578,8 @@
         <v>16059 - 12326</v>
       </c>
       <c r="N61" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16059 - 12326"] +{"Tawny Sabercat", 16059, 12326, 0.6, 0.6, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16059 - 12326"] ={"Tawny Sabercat", 16059, 12326, 0.6, 0.6, 0, "Saber", "removed"},</v>
       </c>
       <c r="O61" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25595,8 +25622,8 @@
         <v>16060 - 12327</v>
       </c>
       <c r="N62" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16060 - 12327"] +{"Golden Sabercat", 16060, 12327, 0.6, 0.6, 0, "Saber", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16060 - 12327"] ={"Golden Sabercat", 16060, 12327, 0.6, 0.6, 0, "Saber", "Removed"},</v>
       </c>
       <c r="O62" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25639,8 +25666,8 @@
         <v>16080 - 12330</v>
       </c>
       <c r="N63" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16080 - 12330"] +{"Red Wolf", 16080, 12330, 1, 1, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16080 - 12330"] ={"Red Wolf", 16080, 12330, 1, 1, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O63" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25683,8 +25710,8 @@
         <v>16081 - 1133</v>
       </c>
       <c r="N64" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16081 - 1133"] +{"Winter Wolf", 16081, 1133, 1, 1, 0, "Wolf", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16081 - 1133"] ={"Winter Wolf", 16081, 1133, 1, 1, 0, "Wolf", "removed"},</v>
       </c>
       <c r="O64" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25727,8 +25754,8 @@
         <v>16082 - 12354</v>
       </c>
       <c r="N65" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16082 - 12354"] +{"Palomino", 16082, 12354, 1, 1, 0, "Horse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16082 - 12354"] ={"Palomino", 16082, 12354, 1, 1, 0, "Horse", "removed"},</v>
       </c>
       <c r="O65" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25774,8 +25801,8 @@
         <v>16083 - 12353</v>
       </c>
       <c r="N66" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16083 - 12353"] +{"White Stallion", 16083, 12353, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16083 - 12353"] ={"White Stallion", 16083, 12353, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O66" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25818,8 +25845,8 @@
         <v>16084 - 8586</v>
       </c>
       <c r="N67" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["16084 - 8586"] +{"Mottled Red Raptor", 16084, 8586, 1, 1, 0, "Raptor", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["16084 - 8586"] ={"Mottled Red Raptor", 16084, 8586, 1, 1, 0, "Raptor", "removed"},</v>
       </c>
       <c r="O67" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25865,8 +25892,8 @@
         <v>17229 - 13086</v>
       </c>
       <c r="N68" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17229 - 13086"] +{"Winterspring Frostsaber", 17229, 13086, 1, 1, 0, "Saber", "Exaulted Winterspring Frostsaber"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17229 - 13086"] ={"Winterspring Frostsaber", 17229, 13086, 1, 1, 0, "Saber", "Exaulted Winterspring Frostsaber"},</v>
       </c>
       <c r="O68" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25909,8 +25936,8 @@
         <v>17450 - 13317</v>
       </c>
       <c r="N69" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17450 - 13317"] +{"Ivory Raptor", 17450, 13317, 1, 1, 0, "Raptor", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17450 - 13317"] ={"Ivory Raptor", 17450, 13317, 1, 1, 0, "Raptor", "Removed"},</v>
       </c>
       <c r="O69" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -25956,8 +25983,8 @@
         <v>17453 - 13321</v>
       </c>
       <c r="N70" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17453 - 13321"] +{"Green Mechanostrider", 17453, 13321, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17453 - 13321"] ={"Green Mechanostrider", 17453, 13321, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O70" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26003,8 +26030,8 @@
         <v>17454 - 13322</v>
       </c>
       <c r="N71" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17454 - 13322"] +{"Unpainted Mechanostrider", 17454, 13322, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17454 - 13322"] ={"Unpainted Mechanostrider", 17454, 13322, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O71" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26047,8 +26074,8 @@
         <v>17455 - 13323</v>
       </c>
       <c r="N72" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17455 - 13323"] +{"Purple Mechanostrider", 17455, 13323, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17455 - 13323"] ={"Purple Mechanostrider", 17455, 13323, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
       </c>
       <c r="O72" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26091,8 +26118,8 @@
         <v>17456 - 13324</v>
       </c>
       <c r="N73" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17456 - 13324"] +{"Red and Blue Mechanostrider", 17456, 13324, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17456 - 13324"] ={"Red and Blue Mechanostrider", 17456, 13324, 0.6, 0.6, 0, "Mechanostrider", "removed"},</v>
       </c>
       <c r="O73" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26135,8 +26162,8 @@
         <v>17458 - 13325</v>
       </c>
       <c r="N74" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17458 - 13325"] +{"Fluorescent Green Mechanostrider", 17458, 13325, 0.6, 0.6, 0, "Mechanostrider", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17458 - 13325"] ={"Fluorescent Green Mechanostrider", 17458, 13325, 0.6, 0.6, 0, "Mechanostrider", "Removed"},</v>
       </c>
       <c r="O74" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26179,8 +26206,8 @@
         <v>17459 - 13327</v>
       </c>
       <c r="N75" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17459 - 13327"] +{"Icy Blue Mechanostrider Mod A", 17459, 13327, 1, 1, 0, "Mechanostrider", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17459 - 13327"] ={"Icy Blue Mechanostrider Mod A", 17459, 13327, 1, 1, 0, "Mechanostrider", "Removed"},</v>
       </c>
       <c r="O75" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26223,8 +26250,8 @@
         <v>17460 - 13329</v>
       </c>
       <c r="N76" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17460 - 13329"] +{"Frost Ram", 17460, 13329, 1, 1, 0, "Ram", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17460 - 13329"] ={"Frost Ram", 17460, 13329, 1, 1, 0, "Ram", "Removed"},</v>
       </c>
       <c r="O76" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26270,8 +26297,8 @@
         <v>17461 - 13328</v>
       </c>
       <c r="N77" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17461 - 13328"] +{"Black Ram", 17461, 13328, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17461 - 13328"] ={"Black Ram", 17461, 13328, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O77" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26314,8 +26341,8 @@
         <v>17462 - 13331</v>
       </c>
       <c r="N78" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17462 - 13331"] +{"Red Skeletal Horse", 17462, 13331, 0.6, 0.6, 0, "Horse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17462 - 13331"] ={"Red Skeletal Horse", 17462, 13331, 0.6, 0.6, 0, "Horse", "Gold"},</v>
       </c>
       <c r="O78" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26358,8 +26385,8 @@
         <v>17463 - 46308</v>
       </c>
       <c r="N79" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17463 - 46308"] +{"Blue Skeletal Horse", 17463, 46308, 0.6, 0.6, 0, "DeadHorse", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17463 - 46308"] ={"Blue Skeletal Horse", 17463, 46308, 0.6, 0.6, 0, "DeadHorse", "Duplicate"},</v>
       </c>
       <c r="O79" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26402,8 +26429,8 @@
         <v>17464 - 13333</v>
       </c>
       <c r="N80" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17464 - 13333"] +{"Brown Skeletal Horse", 17464, 13333, 0.6, 0.6, 0, "Horse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17464 - 13333"] ={"Brown Skeletal Horse", 17464, 13333, 0.6, 0.6, 0, "Horse", "Gold"},</v>
       </c>
       <c r="O80" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26446,8 +26473,8 @@
         <v>17465 - 13334</v>
       </c>
       <c r="N81" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17465 - 13334"] +{"Green Skeletal Warhorse", 17465, 13334, 1, 1, 0, "Horse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17465 - 13334"] ={"Green Skeletal Warhorse", 17465, 13334, 1, 1, 0, "Horse", "Gold"},</v>
       </c>
       <c r="O81" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26496,8 +26523,8 @@
         <v>17481 - 13335</v>
       </c>
       <c r="N82" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["17481 - 13335"] +{"Rivendare's Deathcharger", 17481, 13335, 1, 1, 0, "DeadHorse", "Drop Stratholme"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["17481 - 13335"] ={"Rivendare's Deathcharger", 17481, 13335, 1, 1, 0, "DeadHorse", "Drop Stratholme"},</v>
       </c>
       <c r="O82" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26540,8 +26567,8 @@
         <v>18363 - 14062</v>
       </c>
       <c r="N83" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["18363 - 14062"] +{"Riding Kodo", 18363, 14062, 0.6, 0.6, 0, "Kodo", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["18363 - 14062"] ={"Riding Kodo", 18363, 14062, 0.6, 0.6, 0, "Kodo", "removed"},</v>
       </c>
       <c r="O83" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26584,8 +26611,8 @@
         <v>18989 - 15277</v>
       </c>
       <c r="N84" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["18989 - 15277"] +{"Gray Kodo", 18989, 15277, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["18989 - 15277"] ={"Gray Kodo", 18989, 15277, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O84" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26628,8 +26655,8 @@
         <v>18990 - 15290</v>
       </c>
       <c r="N85" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["18990 - 15290"] +{"Brown Kodo", 18990, 15290, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["18990 - 15290"] ={"Brown Kodo", 18990, 15290, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O85" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26672,8 +26699,8 @@
         <v>18991 - 15292</v>
       </c>
       <c r="N86" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["18991 - 15292"] +{"Green Kodo", 18991, 15292, 1, 1, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["18991 - 15292"] ={"Green Kodo", 18991, 15292, 1, 1, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O86" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26716,8 +26743,8 @@
         <v>18992 - 15293</v>
       </c>
       <c r="N87" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["18992 - 15293"] +{"Teal Kodo", 18992, 15293, 1, 1, 0, "Kodo", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["18992 - 15293"] ={"Teal Kodo", 18992, 15293, 1, 1, 0, "Kodo", "removed"},</v>
       </c>
       <c r="O87" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26760,8 +26787,8 @@
         <v>22717 - 18241</v>
       </c>
       <c r="N88" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22717 - 18241"] +{"Black War Steed", 22717, 18241, 1, 1, 0, "Horse", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22717 - 18241"] ={"Black War Steed", 22717, 18241, 1, 1, 0, "Horse", "Duplicate"},</v>
       </c>
       <c r="O88" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26807,8 +26834,8 @@
         <v>22717 - 29468</v>
       </c>
       <c r="N89" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22717 - 29468"] +{"Black War Steed", 22717, 29468, 1, 1, 0, "Horse", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22717 - 29468"] ={"Black War Steed", 22717, 29468, 1, 1, 0, "Horse", "Honor"},</v>
       </c>
       <c r="O89" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26851,8 +26878,8 @@
         <v>22718 - 18247</v>
       </c>
       <c r="N90" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22718 - 18247"] +{"Black War Kodo", 22718, 18247, 1, 1, 0, "Kodo", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22718 - 18247"] ={"Black War Kodo", 22718, 18247, 1, 1, 0, "Kodo", "Duplicate"},</v>
       </c>
       <c r="O90" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26895,8 +26922,8 @@
         <v>22718 - 29466</v>
       </c>
       <c r="N91" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22718 - 29466"] +{"Black War Kodo", 22718, 29466, 1, 1, 0, "Kodo", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22718 - 29466"] ={"Black War Kodo", 22718, 29466, 1, 1, 0, "Kodo", "Honor"},</v>
       </c>
       <c r="O91" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26939,8 +26966,8 @@
         <v>22719 - 18243</v>
       </c>
       <c r="N92" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22719 - 18243"] +{"Black Battlestrider", 22719, 18243, 1, 1, 0, "Mechanostrider", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22719 - 18243"] ={"Black Battlestrider", 22719, 18243, 1, 1, 0, "Mechanostrider", "Duplicate"},</v>
       </c>
       <c r="O92" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -26986,8 +27013,8 @@
         <v>22719 - 29465</v>
       </c>
       <c r="N93" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22719 - 29465"] +{"Black Battlestrider", 22719, 29465, 1, 1, 0, "Mechanostrider", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22719 - 29465"] ={"Black Battlestrider", 22719, 29465, 1, 1, 0, "Mechanostrider", "Honor"},</v>
       </c>
       <c r="O93" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27030,8 +27057,8 @@
         <v>22720 - 18244</v>
       </c>
       <c r="N94" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22720 - 18244"] +{"Black War Ram", 22720, 18244, 1, 1, 0, "Ram", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22720 - 18244"] ={"Black War Ram", 22720, 18244, 1, 1, 0, "Ram", "Duplicate"},</v>
       </c>
       <c r="O94" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27077,8 +27104,8 @@
         <v>22720 - 29467</v>
       </c>
       <c r="N95" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22720 - 29467"] +{"Black War Ram", 22720, 29467, 1, 1, 0, "Ram", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22720 - 29467"] ={"Black War Ram", 22720, 29467, 1, 1, 0, "Ram", "Honor"},</v>
       </c>
       <c r="O95" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27121,8 +27148,8 @@
         <v>22721 - 18246</v>
       </c>
       <c r="N96" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22721 - 18246"] +{"Black War Raptor", 22721, 18246, 1, 1, 0, "Raptor", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22721 - 18246"] ={"Black War Raptor", 22721, 18246, 1, 1, 0, "Raptor", "Duplicate"},</v>
       </c>
       <c r="O96" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27165,8 +27192,8 @@
         <v>22721 - 29472</v>
       </c>
       <c r="N97" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22721 - 29472"] +{"Black War Raptor", 22721, 29472, 1, 1, 0, "Raptor", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22721 - 29472"] ={"Black War Raptor", 22721, 29472, 1, 1, 0, "Raptor", "Honor"},</v>
       </c>
       <c r="O97" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27209,8 +27236,8 @@
         <v>22722 - 18248</v>
       </c>
       <c r="N98" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22722 - 18248"] +{"Red Skeletal Warhorse", 22722, 18248, 1, 1, 0, "Horse", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22722 - 18248"] ={"Red Skeletal Warhorse", 22722, 18248, 1, 1, 0, "Horse", "Duplicate"},</v>
       </c>
       <c r="O98" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27253,8 +27280,8 @@
         <v>22722 - 29470</v>
       </c>
       <c r="N99" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22722 - 29470"] +{"Red Skeletal Warhorse", 22722, 29470, 1, 1, 0, "Horse", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22722 - 29470"] ={"Red Skeletal Warhorse", 22722, 29470, 1, 1, 0, "Horse", "Honor"},</v>
       </c>
       <c r="O99" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27297,8 +27324,8 @@
         <v>22723 - 18242</v>
       </c>
       <c r="N100" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22723 - 18242"] +{"Black War Tiger", 22723, 18242, 1, 1, 0, "Saber", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22723 - 18242"] ={"Black War Tiger", 22723, 18242, 1, 1, 0, "Saber", "Duplicate"},</v>
       </c>
       <c r="O100" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27344,8 +27371,8 @@
         <v>22723 - 29471</v>
       </c>
       <c r="N101" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22723 - 29471"] +{"Black War Tiger", 22723, 29471, 1, 1, 0, "Saber", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22723 - 29471"] ={"Black War Tiger", 22723, 29471, 1, 1, 0, "Saber", "Honor"},</v>
       </c>
       <c r="O101" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27388,8 +27415,8 @@
         <v>22724 - 18245</v>
       </c>
       <c r="N102" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22724 - 18245"] +{"Black War Wolf", 22724, 18245, 1, 1, 0, "Wolf", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22724 - 18245"] ={"Black War Wolf", 22724, 18245, 1, 1, 0, "Wolf", "Duplicate"},</v>
       </c>
       <c r="O102" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27432,8 +27459,8 @@
         <v>22724 - 29469</v>
       </c>
       <c r="N103" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["22724 - 29469"] +{"Black War Wolf", 22724, 29469, 1, 1, 0, "Wolf", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["22724 - 29469"] ={"Black War Wolf", 22724, 29469, 1, 1, 0, "Wolf", "Honor"},</v>
       </c>
       <c r="O103" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27479,8 +27506,8 @@
         <v>23161 - 0</v>
       </c>
       <c r="N104" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23161 - 0"] +{"Dreadsteed", 23161, 0, 1, 1, 0, "Warlock", "Warlock"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23161 - 0"] ={"Dreadsteed", 23161, 0, 1, 1, 0, "Warlock", "Warlock"},</v>
       </c>
       <c r="O104" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27526,8 +27553,8 @@
         <v>23214 - 0</v>
       </c>
       <c r="N105" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23214 - 0"] +{"Charger", 23214, 0, 1, 1, 0, "Paladin", "Paladin"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23214 - 0"] ={"Charger", 23214, 0, 1, 1, 0, "Paladin", "Paladin"},</v>
       </c>
       <c r="O105" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27573,8 +27600,8 @@
         <v>23219 - 18767</v>
       </c>
       <c r="N106" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23219 - 18767"] +{"Swift Mistsaber", 23219, 18767, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23219 - 18767"] ={"Swift Mistsaber", 23219, 18767, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O106" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27617,8 +27644,8 @@
         <v>23220 - 18768</v>
       </c>
       <c r="N107" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23220 - 18768"] +{"Swift Dawnsaber", 23220, 18768, 1, 1, 0, "Saber", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23220 - 18768"] ={"Swift Dawnsaber", 23220, 18768, 1, 1, 0, "Saber", "removed"},</v>
       </c>
       <c r="O107" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27664,8 +27691,8 @@
         <v>23221 - 18766</v>
       </c>
       <c r="N108" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23221 - 18766"] +{"Swift Frostsaber", 23221, 18766, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23221 - 18766"] ={"Swift Frostsaber", 23221, 18766, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O108" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27711,8 +27738,8 @@
         <v>23222 - 18774</v>
       </c>
       <c r="N109" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23222 - 18774"] +{"Swift Yellow Mechanostrider", 23222, 18774, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23222 - 18774"] ={"Swift Yellow Mechanostrider", 23222, 18774, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O109" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27758,8 +27785,8 @@
         <v>23223 - 18773</v>
       </c>
       <c r="N110" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23223 - 18773"] +{"Swift White Mechanostrider", 23223, 18773, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23223 - 18773"] ={"Swift White Mechanostrider", 23223, 18773, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O110" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27805,8 +27832,8 @@
         <v>23225 - 18772</v>
       </c>
       <c r="N111" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23225 - 18772"] +{"Swift Green Mechanostrider", 23225, 18772, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23225 - 18772"] ={"Swift Green Mechanostrider", 23225, 18772, 1, 1, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O111" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27852,8 +27879,8 @@
         <v>23227 - 18776</v>
       </c>
       <c r="N112" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23227 - 18776"] +{"Swift Palomino", 23227, 18776, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23227 - 18776"] ={"Swift Palomino", 23227, 18776, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O112" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27899,8 +27926,8 @@
         <v>23228 - 18778</v>
       </c>
       <c r="N113" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23228 - 18778"] +{"Swift White Steed", 23228, 18778, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23228 - 18778"] ={"Swift White Steed", 23228, 18778, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O113" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27946,8 +27973,8 @@
         <v>23229 - 18777</v>
       </c>
       <c r="N114" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23229 - 18777"] +{"Swift Brown Steed", 23229, 18777, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23229 - 18777"] ={"Swift Brown Steed", 23229, 18777, 1, 1, 0, "Horse", "Exaulted Stormwind"},</v>
       </c>
       <c r="O114" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -27993,8 +28020,8 @@
         <v>23238 - 18786</v>
       </c>
       <c r="N115" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23238 - 18786"] +{"Swift Brown Ram", 23238, 18786, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23238 - 18786"] ={"Swift Brown Ram", 23238, 18786, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O115" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28040,8 +28067,8 @@
         <v>23239 - 18787</v>
       </c>
       <c r="N116" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23239 - 18787"] +{"Swift Gray Ram", 23239, 18787, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23239 - 18787"] ={"Swift Gray Ram", 23239, 18787, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O116" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28087,8 +28114,8 @@
         <v>23240 - 18785</v>
       </c>
       <c r="N117" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23240 - 18785"] +{"Swift White Ram", 23240, 18785, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23240 - 18785"] ={"Swift White Ram", 23240, 18785, 1, 1, 0, "Ram", "Exaulted IronForge"},</v>
       </c>
       <c r="O117" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28131,8 +28158,8 @@
         <v>23241 - 18788</v>
       </c>
       <c r="N118" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23241 - 18788"] +{"Swift Blue Raptor", 23241, 18788, 1, 1, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23241 - 18788"] ={"Swift Blue Raptor", 23241, 18788, 1, 1, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O118" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28175,8 +28202,8 @@
         <v>23242 - 18789</v>
       </c>
       <c r="N119" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23242 - 18789"] +{"Swift Olive Raptor", 23242, 18789, 1, 1, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23242 - 18789"] ={"Swift Olive Raptor", 23242, 18789, 1, 1, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O119" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28219,8 +28246,8 @@
         <v>23243 - 18790</v>
       </c>
       <c r="N120" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23243 - 18790"] +{"Swift Orange Raptor", 23243, 18790, 1, 1, 0, "Raptor", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23243 - 18790"] ={"Swift Orange Raptor", 23243, 18790, 1, 1, 0, "Raptor", "Gold"},</v>
       </c>
       <c r="O120" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28263,8 +28290,8 @@
         <v>23246 - 18791</v>
       </c>
       <c r="N121" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23246 - 18791"] +{"Purple Skeletal Warhorse", 23246, 18791, 1, 1, 0, "Horse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23246 - 18791"] ={"Purple Skeletal Warhorse", 23246, 18791, 1, 1, 0, "Horse", "Gold"},</v>
       </c>
       <c r="O121" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28307,8 +28334,8 @@
         <v>23247 - 18793</v>
       </c>
       <c r="N122" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23247 - 18793"] +{"Great White Kodo", 23247, 18793, 1, 1, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23247 - 18793"] ={"Great White Kodo", 23247, 18793, 1, 1, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O122" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28351,8 +28378,8 @@
         <v>23248 - 18795</v>
       </c>
       <c r="N123" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23248 - 18795"] +{"Great Gray Kodo", 23248, 18795, 1, 1, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23248 - 18795"] ={"Great Gray Kodo", 23248, 18795, 1, 1, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O123" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28395,8 +28422,8 @@
         <v>23249 - 18794</v>
       </c>
       <c r="N124" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23249 - 18794"] +{"Great Brown Kodo", 23249, 18794, 1, 1, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23249 - 18794"] ={"Great Brown Kodo", 23249, 18794, 1, 1, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O124" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28439,8 +28466,8 @@
         <v>23250 - 18796</v>
       </c>
       <c r="N125" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23250 - 18796"] +{"Swift Brown Wolf", 23250, 18796, 1, 1, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23250 - 18796"] ={"Swift Brown Wolf", 23250, 18796, 1, 1, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O125" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28483,8 +28510,8 @@
         <v>23251 - 18797</v>
       </c>
       <c r="N126" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23251 - 18797"] +{"Swift Timber Wolf", 23251, 18797, 1, 1, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23251 - 18797"] ={"Swift Timber Wolf", 23251, 18797, 1, 1, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O126" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28527,8 +28554,8 @@
         <v>23252 - 1134</v>
       </c>
       <c r="N127" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23252 - 1134"] +{"Swift Gray Wolf", 23252, 1134, 1, 1, 0, "Wolf", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23252 - 1134"] ={"Swift Gray Wolf", 23252, 1134, 1, 1, 0, "Wolf", "Duplicate"},</v>
       </c>
       <c r="O127" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28571,8 +28598,8 @@
         <v>23252 - 18798</v>
       </c>
       <c r="N128" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23252 - 18798"] +{"Swift Gray Wolf", 23252, 18798, 1, 1, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23252 - 18798"] ={"Swift Gray Wolf", 23252, 18798, 1, 1, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O128" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28618,8 +28645,8 @@
         <v>23338 - 18902</v>
       </c>
       <c r="N129" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23338 - 18902"] +{"Swift Stormsaber", 23338, 18902, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23338 - 18902"] ={"Swift Stormsaber", 23338, 18902, 1, 1, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O129" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28662,8 +28689,8 @@
         <v>23509 - 19029</v>
       </c>
       <c r="N130" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23509 - 19029"] +{"Frostwolf Howler", 23509, 19029, 1, 1, 0, "Wolf", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23509 - 19029"] ={"Frostwolf Howler", 23509, 19029, 1, 1, 0, "Wolf", "Honor"},</v>
       </c>
       <c r="O130" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28709,8 +28736,8 @@
         <v>23510 - 19030</v>
       </c>
       <c r="N131" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["23510 - 19030"] +{"Stormpike Battle Charger", 23510, 19030, 1, 1, 0, "Ram", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["23510 - 19030"] ={"Stormpike Battle Charger", 23510, 19030, 1, 1, 0, "Ram", "Honor"},</v>
       </c>
       <c r="O131" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28759,8 +28786,8 @@
         <v>24242 - 19872</v>
       </c>
       <c r="N132" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["24242 - 19872"] +{"Swift Razzashi Raptor", 24242, 19872, 1, 1, 0, "Raptor", "Drop ZG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["24242 - 19872"] ={"Swift Razzashi Raptor", 24242, 19872, 1, 1, 0, "Raptor", "Drop ZG"},</v>
       </c>
       <c r="O132" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28809,8 +28836,8 @@
         <v>24252 - 19902</v>
       </c>
       <c r="N133" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["24252 - 19902"] +{"Swift Zulian Tiger", 24252, 19902, 1, 1, 0, "Saber", "Drop ZG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["24252 - 19902"] ={"Swift Zulian Tiger", 24252, 19902, 1, 1, 0, "Saber", "Drop ZG"},</v>
       </c>
       <c r="O133" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28859,8 +28886,8 @@
         <v>25953 - 21218</v>
       </c>
       <c r="N134" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["25953 - 21218"] +{"Blue Qiraji Battle Tank", 25953, 21218, 1, 1, 0, "Bug", "Drop, AQ40"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["25953 - 21218"] ={"Blue Qiraji Battle Tank", 25953, 21218, 1, 1, 0, "Bug", "Drop, AQ40"},</v>
       </c>
       <c r="O134" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28909,8 +28936,8 @@
         <v>26054 - 21321</v>
       </c>
       <c r="N135" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["26054 - 21321"] +{"Red Qiraji Battle Tank", 26054, 21321, 1, 1, 0, "Bug", "Drop AQ40"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["26054 - 21321"] ={"Red Qiraji Battle Tank", 26054, 21321, 1, 1, 0, "Bug", "Drop AQ40"},</v>
       </c>
       <c r="O135" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -28959,8 +28986,8 @@
         <v>26055 - 21324</v>
       </c>
       <c r="N136" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["26055 - 21324"] +{"Yellow Qiraji Battle Tank", 26055, 21324, 1, 1, 0, "Bug", "Drop AQ40"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["26055 - 21324"] ={"Yellow Qiraji Battle Tank", 26055, 21324, 1, 1, 0, "Bug", "Drop AQ40"},</v>
       </c>
       <c r="O136" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29009,8 +29036,8 @@
         <v>26056 - 21323</v>
       </c>
       <c r="N137" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["26056 - 21323"] +{"Green Qiraji Battle Tank", 26056, 21323, 1, 1, 0, "Bug", "Drop AQ40"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["26056 - 21323"] ={"Green Qiraji Battle Tank", 26056, 21323, 1, 1, 0, "Bug", "Drop AQ40"},</v>
       </c>
       <c r="O137" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29056,8 +29083,8 @@
         <v>26656 - 21176</v>
       </c>
       <c r="N138" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["26656 - 21176"] +{"Black Qiraji Battle Tank", 26656, 21176, 1, 1, 0, "Bug", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["26656 - 21176"] ={"Black Qiraji Battle Tank", 26656, 21176, 1, 1, 0, "Bug", "Removed"},</v>
       </c>
       <c r="O138" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29103,8 +29130,8 @@
         <v>28825 - 21736</v>
       </c>
       <c r="N139" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["28825 - 21736"] +{"Nether Drake", 28825, 21736, 3, 3, 0, "Nether Drake", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["28825 - 21736"] ={"Nether Drake", 28825, 21736, 3, 3, 0, "Nether Drake", "removed"},</v>
       </c>
       <c r="O139" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29147,8 +29174,8 @@
         <v>29059 - 23193</v>
       </c>
       <c r="N140" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["29059 - 23193"] +{"Naxxramas Deathcharger", 29059, 23193, 1, 1, 0, "DeadHorse", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["29059 - 23193"] ={"Naxxramas Deathcharger", 29059, 23193, 1, 1, 0, "DeadHorse", "removed"},</v>
       </c>
       <c r="O140" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29194,8 +29221,8 @@
         <v>30174 - 23720</v>
       </c>
       <c r="N141" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["30174 - 23720"] +{"Riding Turtle", 30174, 23720, 0, 0, 1, "Turtle", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["30174 - 23720"] ={"Riding Turtle", 30174, 23720, 0, 0, 1, "Turtle", "TCG"},</v>
       </c>
       <c r="O141" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29241,8 +29268,8 @@
         <v>32235 - 25470</v>
       </c>
       <c r="N142" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32235 - 25470"] +{"Golden Gryphon", 32235, 25470, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32235 - 25470"] ={"Golden Gryphon", 32235, 25470, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O142" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29288,8 +29315,8 @@
         <v>32239 - 25471</v>
       </c>
       <c r="N143" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32239 - 25471"] +{"Ebon Gryphon", 32239, 25471, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32239 - 25471"] ={"Ebon Gryphon", 32239, 25471, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O143" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29335,8 +29362,8 @@
         <v>32240 - 25472</v>
       </c>
       <c r="N144" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32240 - 25472"] +{"Snowy Gryphon", 32240, 25472, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32240 - 25472"] ={"Snowy Gryphon", 32240, 25472, 1.5, 1.5, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O144" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29382,8 +29409,8 @@
         <v>32242 - 25473</v>
       </c>
       <c r="N145" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32242 - 25473"] +{"Swift Blue Gryphon", 32242, 25473, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32242 - 25473"] ={"Swift Blue Gryphon", 32242, 25473, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O145" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29426,8 +29453,8 @@
         <v>32243 - 25474</v>
       </c>
       <c r="N146" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32243 - 25474"] +{"Tawny Wind Rider", 32243, 25474, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32243 - 25474"] ={"Tawny Wind Rider", 32243, 25474, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O146" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29470,8 +29497,8 @@
         <v>32244 - 25475</v>
       </c>
       <c r="N147" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32244 - 25475"] +{"Blue Wind Rider", 32244, 25475, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32244 - 25475"] ={"Blue Wind Rider", 32244, 25475, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O147" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29514,8 +29541,8 @@
         <v>32245 - 25476</v>
       </c>
       <c r="N148" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32245 - 25476"] +{"Green Wind Rider", 32245, 25476, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32245 - 25476"] ={"Green Wind Rider", 32245, 25476, 1.5, 1.5, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O148" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29558,8 +29585,8 @@
         <v>32246 - 25477</v>
       </c>
       <c r="N149" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32246 - 25477"] +{"Swift Red Wind Rider", 32246, 25477, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32246 - 25477"] ={"Swift Red Wind Rider", 32246, 25477, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O149" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29605,8 +29632,8 @@
         <v>32289 - 25527</v>
       </c>
       <c r="N150" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32289 - 25527"] +{"Swift Red Gryphon", 32289, 25527, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32289 - 25527"] ={"Swift Red Gryphon", 32289, 25527, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O150" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29652,8 +29679,8 @@
         <v>32290 - 25528</v>
       </c>
       <c r="N151" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32290 - 25528"] +{"Swift Green Gryphon", 32290, 25528, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32290 - 25528"] ={"Swift Green Gryphon", 32290, 25528, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O151" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29699,8 +29726,8 @@
         <v>32292 - 25529</v>
       </c>
       <c r="N152" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32292 - 25529"] +{"Swift Purple Gryphon", 32292, 25529, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32292 - 25529"] ={"Swift Purple Gryphon", 32292, 25529, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O152" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29743,8 +29770,8 @@
         <v>32295 - 25531</v>
       </c>
       <c r="N153" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32295 - 25531"] +{"Swift Green Wind Rider", 32295, 25531, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32295 - 25531"] ={"Swift Green Wind Rider", 32295, 25531, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O153" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29787,8 +29814,8 @@
         <v>32296 - 25532</v>
       </c>
       <c r="N154" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32296 - 25532"] +{"Swift Yellow Wind Rider", 32296, 25532, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32296 - 25532"] ={"Swift Yellow Wind Rider", 32296, 25532, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O154" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29831,8 +29858,8 @@
         <v>32297 - 25533</v>
       </c>
       <c r="N155" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32297 - 25533"] +{"Swift Purple Wind Rider", 32297, 25533, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32297 - 25533"] ={"Swift Purple Wind Rider", 32297, 25533, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O155" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29878,8 +29905,8 @@
         <v>32345 - 25596</v>
       </c>
       <c r="N156" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32345 - 25596"] +{"Peep the Phoenix Mount", 32345, 25596, 3.1, 3.1, 0, "Phoenix", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32345 - 25596"] ={"Peep the Phoenix Mount", 32345, 25596, 3.1, 3.1, 0, "Phoenix", "removed"},</v>
       </c>
       <c r="O156" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29922,8 +29949,8 @@
         <v>32420 - 25664</v>
       </c>
       <c r="N157" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["32420 - 25664"] +{"Old Crappy McWeakSauce", 32420, 25664, 0.6, 0.6, 0, "Wind Rider", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["32420 - 25664"] ={"Old Crappy McWeakSauce", 32420, 25664, 0.6, 0.6, 0, "Wind Rider", "removed"},</v>
       </c>
       <c r="O157" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -29969,8 +29996,8 @@
         <v>33630 - 8595</v>
       </c>
       <c r="N158" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["33630 - 8595"] +{"Blue Mechanostrider", 33630, 8595, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["33630 - 8595"] ={"Blue Mechanostrider", 33630, 8595, 0.6, 0.6, 0, "Mechanostrider", "Exaulted Gnomeragan"},</v>
       </c>
       <c r="O158" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30013,8 +30040,8 @@
         <v>33660 - 28936</v>
       </c>
       <c r="N159" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["33660 - 28936"] +{"Swift Pink Hawkstrider", 33660, 28936, 1, 1, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["33660 - 28936"] ={"Swift Pink Hawkstrider", 33660, 28936, 1, 1, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O159" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30060,8 +30087,8 @@
         <v>34406 - 28481</v>
       </c>
       <c r="N160" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34406 - 28481"] +{"Brown Elekk", 34406, 28481, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34406 - 28481"] ={"Brown Elekk", 34406, 28481, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O160" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30107,8 +30134,8 @@
         <v>34407 - 28482</v>
       </c>
       <c r="N161" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34407 - 28482"] +{"Great Elite Elekk", 34407, 28482, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34407 - 28482"] ={"Great Elite Elekk", 34407, 28482, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O161" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30154,8 +30181,8 @@
         <v>34767 - 0</v>
       </c>
       <c r="N162" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34767 - 0"] +{"Summon Charger", 34767, 0, 1, 1, 0, "Paladin", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34767 - 0"] ={"Summon Charger", 34767, 0, 1, 1, 0, "Paladin", "Duplicate"},</v>
       </c>
       <c r="O162" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30201,8 +30228,8 @@
         <v>34769 - 0</v>
       </c>
       <c r="N163" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34769 - 0"] +{"Summon Warhorse", 34769, 0, 0.6, 0.6, 0, "Paladin", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34769 - 0"] ={"Summon Warhorse", 34769, 0, 0.6, 0.6, 0, "Paladin", "Duplicate"},</v>
       </c>
       <c r="O163" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30251,8 +30278,8 @@
         <v>34790 - 29228</v>
       </c>
       <c r="N164" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34790 - 29228"] +{"Dark War Talbuk", 34790, 29228, 1, 1, 0, "Talbuk", "Hala tokens"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34790 - 29228"] ={"Dark War Talbuk", 34790, 29228, 1, 1, 0, "Talbuk", "Hala tokens"},</v>
       </c>
       <c r="O164" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30295,8 +30322,8 @@
         <v>34795 - 28927</v>
       </c>
       <c r="N165" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34795 - 28927"] +{"Red Hawkstrider", 34795, 28927, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34795 - 28927"] ={"Red Hawkstrider", 34795, 28927, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O165" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30339,8 +30366,8 @@
         <v>34896 - 29102</v>
       </c>
       <c r="N166" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34896 - 29102"] +{"Cobalt War Talbuk", 34896, 29102, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34896 - 29102"] ={"Cobalt War Talbuk", 34896, 29102, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O166" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30386,8 +30413,8 @@
         <v>34896 - 29227</v>
       </c>
       <c r="N167" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34896 - 29227"] +{"Cobalt War Talbuk", 34896, 29227, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34896 - 29227"] ={"Cobalt War Talbuk", 34896, 29227, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O167" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30430,8 +30457,8 @@
         <v>34897 - 29103</v>
       </c>
       <c r="N168" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34897 - 29103"] +{"White War Talbuk", 34897, 29103, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34897 - 29103"] ={"White War Talbuk", 34897, 29103, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O168" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30477,8 +30504,8 @@
         <v>34897 - 29231</v>
       </c>
       <c r="N169" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34897 - 29231"] +{"White War Talbuk", 34897, 29231, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34897 - 29231"] ={"White War Talbuk", 34897, 29231, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O169" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30521,8 +30548,8 @@
         <v>34898 - 29104</v>
       </c>
       <c r="N170" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34898 - 29104"] +{"Silver War Talbuk", 34898, 29104, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34898 - 29104"] ={"Silver War Talbuk", 34898, 29104, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O170" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30568,8 +30595,8 @@
         <v>34898 - 29229</v>
       </c>
       <c r="N171" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34898 - 29229"] +{"Silver War Talbuk", 34898, 29229, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34898 - 29229"] ={"Silver War Talbuk", 34898, 29229, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O171" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30612,8 +30639,8 @@
         <v>34899 - 29105</v>
       </c>
       <c r="N172" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34899 - 29105"] +{"Tan War Talbuk", 34899, 29105, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34899 - 29105"] ={"Tan War Talbuk", 34899, 29105, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O172" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30659,8 +30686,8 @@
         <v>34899 - 29230</v>
       </c>
       <c r="N173" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["34899 - 29230"] +{"Tan War Talbuk", 34899, 29230, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["34899 - 29230"] ={"Tan War Talbuk", 34899, 29230, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O173" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30703,8 +30730,8 @@
         <v>35018 - 29222</v>
       </c>
       <c r="N174" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35018 - 29222"] +{"Purple Hawkstrider", 35018, 29222, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35018 - 29222"] ={"Purple Hawkstrider", 35018, 29222, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O174" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30747,8 +30774,8 @@
         <v>35020 - 29220</v>
       </c>
       <c r="N175" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35020 - 29220"] +{"Blue Hawkstrider", 35020, 29220, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35020 - 29220"] ={"Blue Hawkstrider", 35020, 29220, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O175" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30791,8 +30818,8 @@
         <v>35022 - 29221</v>
       </c>
       <c r="N176" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35022 - 29221"] +{"Black Hawkstrider", 35022, 29221, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35022 - 29221"] ={"Black Hawkstrider", 35022, 29221, 0.6, 0.6, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O176" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30835,8 +30862,8 @@
         <v>35025 - 29223</v>
       </c>
       <c r="N177" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35025 - 29223"] +{"Swift Green Hawkstrider", 35025, 29223, 1, 1, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35025 - 29223"] ={"Swift Green Hawkstrider", 35025, 29223, 1, 1, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O177" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30879,8 +30906,8 @@
         <v>35027 - 29224</v>
       </c>
       <c r="N178" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35027 - 29224"] +{"Swift Purple Hawkstrider", 35027, 29224, 1, 1, 0, "Hawkstrider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35027 - 29224"] ={"Swift Purple Hawkstrider", 35027, 29224, 1, 1, 0, "Hawkstrider", "Gold"},</v>
       </c>
       <c r="O178" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30923,8 +30950,8 @@
         <v>35028 - 34129</v>
       </c>
       <c r="N179" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35028 - 34129"] +{"Swift Warstrider", 35028, 34129, 1, 1, 0, "Hawkstrider", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35028 - 34129"] ={"Swift Warstrider", 35028, 34129, 1, 1, 0, "Hawkstrider", "Honor"},</v>
       </c>
       <c r="O179" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -30970,8 +30997,8 @@
         <v>35710 - 29744</v>
       </c>
       <c r="N180" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35710 - 29744"] +{"Gray Elekk", 35710, 29744, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35710 - 29744"] ={"Gray Elekk", 35710, 29744, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O180" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31017,8 +31044,8 @@
         <v>35711 - 29743</v>
       </c>
       <c r="N181" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35711 - 29743"] +{"Purple Elekk", 35711, 29743, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35711 - 29743"] ={"Purple Elekk", 35711, 29743, 0.6, 0.6, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O181" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31064,8 +31091,8 @@
         <v>35712 - 29746</v>
       </c>
       <c r="N182" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35712 - 29746"] +{"Great Green Elekk", 35712, 29746, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35712 - 29746"] ={"Great Green Elekk", 35712, 29746, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O182" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31111,8 +31138,8 @@
         <v>35713 - 29745</v>
       </c>
       <c r="N183" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35713 - 29745"] +{"Great Blue Elekk", 35713, 29745, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35713 - 29745"] ={"Great Blue Elekk", 35713, 29745, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O183" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31158,8 +31185,8 @@
         <v>35714 - 29747</v>
       </c>
       <c r="N184" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["35714 - 29747"] +{"Great Purple Elekk", 35714, 29747, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["35714 - 29747"] ={"Great Purple Elekk", 35714, 29747, 1, 1, 0, "Elekk", "Exaulted Exodar"},</v>
       </c>
       <c r="O184" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31208,8 +31235,8 @@
         <v>36702 - 30480</v>
       </c>
       <c r="N185" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["36702 - 30480"] +{"Fiery Warhorse", 36702, 30480, 1, 1, 0, "Horse", "Drop Kara"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["36702 - 30480"] ={"Fiery Warhorse", 36702, 30480, 1, 1, 0, "Horse", "Drop Kara"},</v>
       </c>
       <c r="O185" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31255,8 +31282,8 @@
         <v>37015 - 30609</v>
       </c>
       <c r="N186" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["37015 - 30609"] +{"Swift Nether Drake", 37015, 30609, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["37015 - 30609"] ={"Swift Nether Drake", 37015, 30609, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
       </c>
       <c r="O186" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31299,8 +31326,8 @@
         <v>39315 - 31829</v>
       </c>
       <c r="N187" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39315 - 31829"] +{"Cobalt Riding Talbuk", 39315, 31829, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39315 - 31829"] ={"Cobalt Riding Talbuk", 39315, 31829, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O187" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31346,8 +31373,8 @@
         <v>39315 - 31830</v>
       </c>
       <c r="N188" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39315 - 31830"] +{"Cobalt Riding Talbuk", 39315, 31830, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39315 - 31830"] ={"Cobalt Riding Talbuk", 39315, 31830, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O188" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31396,8 +31423,8 @@
         <v>39316 - 28915</v>
       </c>
       <c r="N189" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39316 - 28915"] +{"Dark Riding Talbuk", 39316, 28915, 1, 1, 0, "Talbuk", "Hala tokens"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39316 - 28915"] ={"Dark Riding Talbuk", 39316, 28915, 1, 1, 0, "Talbuk", "Hala tokens"},</v>
       </c>
       <c r="O189" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31440,8 +31467,8 @@
         <v>39317 - 31831</v>
       </c>
       <c r="N190" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39317 - 31831"] +{"Silver Riding Talbuk", 39317, 31831, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39317 - 31831"] ={"Silver Riding Talbuk", 39317, 31831, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O190" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31487,8 +31514,8 @@
         <v>39317 - 31832</v>
       </c>
       <c r="N191" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39317 - 31832"] +{"Silver Riding Talbuk", 39317, 31832, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39317 - 31832"] ={"Silver Riding Talbuk", 39317, 31832, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O191" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31531,8 +31558,8 @@
         <v>39318 - 31833</v>
       </c>
       <c r="N192" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39318 - 31833"] +{"Tan Riding Talbuk", 39318, 31833, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39318 - 31833"] ={"Tan Riding Talbuk", 39318, 31833, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O192" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31578,8 +31605,8 @@
         <v>39318 - 31834</v>
       </c>
       <c r="N193" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39318 - 31834"] +{"Tan Riding Talbuk", 39318, 31834, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39318 - 31834"] ={"Tan Riding Talbuk", 39318, 31834, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O193" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31622,8 +31649,8 @@
         <v>39319 - 31835</v>
       </c>
       <c r="N194" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39319 - 31835"] +{"White Riding Talbuk", 39319, 31835, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39319 - 31835"] ={"White Riding Talbuk", 39319, 31835, 1, 1, 0, "Talbuk", "Mag'har Exaulted"},</v>
       </c>
       <c r="O194" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31669,8 +31696,8 @@
         <v>39319 - 31836</v>
       </c>
       <c r="N195" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39319 - 31836"] +{"White Riding Talbuk", 39319, 31836, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39319 - 31836"] ={"White Riding Talbuk", 39319, 31836, 1, 1, 0, "Talbuk", "Exaulted Kurenai"},</v>
       </c>
       <c r="O195" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31719,8 +31746,8 @@
         <v>39798 - 32314</v>
       </c>
       <c r="N196" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39798 - 32314"] +{"Green Riding Nether Ray", 39798, 32314, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39798 - 32314"] ={"Green Riding Nether Ray", 39798, 32314, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
       </c>
       <c r="O196" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31769,8 +31796,8 @@
         <v>39800 - 32317</v>
       </c>
       <c r="N197" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39800 - 32317"] +{"Red Riding Nether Ray", 39800, 32317, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39800 - 32317"] ={"Red Riding Nether Ray", 39800, 32317, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
       </c>
       <c r="O197" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31819,8 +31846,8 @@
         <v>39801 - 32316</v>
       </c>
       <c r="N198" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39801 - 32316"] +{"Purple Riding Nether Ray", 39801, 32316, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39801 - 32316"] ={"Purple Riding Nether Ray", 39801, 32316, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
       </c>
       <c r="O198" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31869,8 +31896,8 @@
         <v>39802 - 32318</v>
       </c>
       <c r="N199" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39802 - 32318"] +{"Silver Riding Nether Ray", 39802, 32318, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39802 - 32318"] ={"Silver Riding Nether Ray", 39802, 32318, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
       </c>
       <c r="O199" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31919,8 +31946,8 @@
         <v>39803 - 32319</v>
       </c>
       <c r="N200" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["39803 - 32319"] +{"Blue Riding Nether Ray", 39803, 32319, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["39803 - 32319"] ={"Blue Riding Nether Ray", 39803, 32319, 2.8, 2.8, 0, "Nether Ray", "Exaulted Skyguard"},</v>
       </c>
       <c r="O200" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -31969,8 +31996,8 @@
         <v>40192 - 32458</v>
       </c>
       <c r="N201" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["40192 - 32458"] +{"Ashes of Al'ar", 40192, 32458, 3.1, 3.1, 0, "Phoenix", "Drop Tempest Keep"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["40192 - 32458"] ={"Ashes of Al'ar", 40192, 32458, 3.1, 3.1, 0, "Phoenix", "Drop Tempest Keep"},</v>
       </c>
       <c r="O201" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32019,8 +32046,8 @@
         <v>41252 - 32768</v>
       </c>
       <c r="N202" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41252 - 32768"] +{"Raven Lord", 41252, 32768, 1, 1, 0, "Raven", "Drop Sethekk Halls"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41252 - 32768"] ={"Raven Lord", 41252, 32768, 1, 1, 0, "Raven", "Drop Sethekk Halls"},</v>
       </c>
       <c r="O202" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32069,8 +32096,8 @@
         <v>41513 - 32857</v>
       </c>
       <c r="N203" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41513 - 32857"] +{"Onyx Netherwing Drake", 41513, 32857, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41513 - 32857"] ={"Onyx Netherwing Drake", 41513, 32857, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O203" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32119,8 +32146,8 @@
         <v>41514 - 32858</v>
       </c>
       <c r="N204" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41514 - 32858"] +{"Azure Netherwing Drake", 41514, 32858, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41514 - 32858"] ={"Azure Netherwing Drake", 41514, 32858, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O204" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32169,8 +32196,8 @@
         <v>41515 - 32859</v>
       </c>
       <c r="N205" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41515 - 32859"] +{"Cobalt Netherwing Drake", 41515, 32859, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41515 - 32859"] ={"Cobalt Netherwing Drake", 41515, 32859, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O205" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32219,8 +32246,8 @@
         <v>41516 - 32860</v>
       </c>
       <c r="N206" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41516 - 32860"] +{"Purple Netherwing Drake", 41516, 32860, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41516 - 32860"] ={"Purple Netherwing Drake", 41516, 32860, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O206" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32269,8 +32296,8 @@
         <v>41517 - 32861</v>
       </c>
       <c r="N207" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41517 - 32861"] +{"Veridian Netherwing Drake", 41517, 32861, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41517 - 32861"] ={"Veridian Netherwing Drake", 41517, 32861, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O207" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32319,8 +32346,8 @@
         <v>41518 - 32862</v>
       </c>
       <c r="N208" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["41518 - 32862"] +{"Violet Netherwing Drake", 41518, 32862, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["41518 - 32862"] ={"Violet Netherwing Drake", 41518, 32862, 2.8, 2.8, 0, "Nether Drake", "Exaulted Netherwing"},</v>
       </c>
       <c r="O208" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32366,8 +32393,8 @@
         <v>42776 - 33224</v>
       </c>
       <c r="N209" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["42776 - 33224"] +{"Spectral Tiger", 42776, 33224, 0.6, 0.6, 0, "Saber", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["42776 - 33224"] ={"Spectral Tiger", 42776, 33224, 0.6, 0.6, 0, "Saber", "Duplicate"},</v>
       </c>
       <c r="O209" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32413,8 +32440,8 @@
         <v>42776 - 49283</v>
       </c>
       <c r="N210" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["42776 - 49283"] +{"Spectral Tiger", 42776, 49283, 0.6, 0.6, 0, "Saber", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["42776 - 49283"] ={"Spectral Tiger", 42776, 49283, 0.6, 0.6, 0, "Saber", "TCG"},</v>
       </c>
       <c r="O210" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32460,8 +32487,8 @@
         <v>42777 - 33225</v>
       </c>
       <c r="N211" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["42777 - 33225"] +{"Swift Spectral Tiger", 42777, 33225, 1, 1, 0, "Saber", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["42777 - 33225"] ={"Swift Spectral Tiger", 42777, 33225, 1, 1, 0, "Saber", "Duplicate"},</v>
       </c>
       <c r="O211" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32507,8 +32534,8 @@
         <v>42777 - 49284</v>
       </c>
       <c r="N212" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["42777 - 49284"] +{"Swift Spectral Tiger", 42777, 49284, 1, 1, 0, "Saber", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["42777 - 49284"] ={"Swift Spectral Tiger", 42777, 49284, 1, 1, 0, "Saber", "TCG"},</v>
       </c>
       <c r="O212" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32557,8 +32584,8 @@
         <v>43688 - 33809</v>
       </c>
       <c r="N213" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["43688 - 33809"] +{"Amani War Bear", 43688, 33809, 1, 1, 0, "Bear", "ZA"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["43688 - 33809"] ={"Amani War Bear", 43688, 33809, 1, 1, 0, "Bear", "ZA"},</v>
       </c>
       <c r="O213" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32604,8 +32631,8 @@
         <v>43810 - 0</v>
       </c>
       <c r="N214" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["43810 - 0"] +{"Frost Wyrm", 43810, 0, 2.8, 2.8, 0, "Wyrm", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["43810 - 0"] ={"Frost Wyrm", 43810, 0, 2.8, 2.8, 0, "Wyrm", "Removed"},</v>
       </c>
       <c r="O214" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32651,8 +32678,8 @@
         <v>43899 - 33976</v>
       </c>
       <c r="N215" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["43899 - 33976"] +{"Brewfest Ram", 43899, 33976, 0.6, 0.6, 0, "Ram", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["43899 - 33976"] ={"Brewfest Ram", 43899, 33976, 0.6, 0.6, 0, "Ram", "Duplicate"},</v>
       </c>
       <c r="O215" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32701,8 +32728,8 @@
         <v>43900 - 33977</v>
       </c>
       <c r="N216" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["43900 - 33977"] +{"Swift Brewfest Ram", 43900, 33977, 1, 1, 0, "Ram", "Drop Brewfest"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["43900 - 33977"] ={"Swift Brewfest Ram", 43900, 33977, 1, 1, 0, "Ram", "Drop Brewfest"},</v>
       </c>
       <c r="O216" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32751,8 +32778,8 @@
         <v>43927 - 33999</v>
       </c>
       <c r="N217" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["43927 - 33999"] +{"Cenarion War Hippogryph", 43927, 33999, 2.8, 2.8, 0, "Hippogryph", "Exaulted Cenarion Expedition"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["43927 - 33999"] ={"Cenarion War Hippogryph", 43927, 33999, 2.8, 2.8, 0, "Hippogryph", "Exaulted Cenarion Expedition"},</v>
       </c>
       <c r="O217" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32801,8 +32828,8 @@
         <v>44151 - 34061</v>
       </c>
       <c r="N218" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["44151 - 34061"] +{"Turbo-Charged Flying Machine", 44151, 34061, 2.8, 2.8, 0, "Machine", "Engineering"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["44151 - 34061"] ={"Turbo-Charged Flying Machine", 44151, 34061, 2.8, 2.8, 0, "Machine", "Engineering"},</v>
       </c>
       <c r="O218" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32851,8 +32878,8 @@
         <v>44153 - 34060</v>
       </c>
       <c r="N219" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["44153 - 34060"] +{"Flying Machine", 44153, 34060, 1.5, 1.5, 0, "Machine", "Engineering"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["44153 - 34060"] ={"Flying Machine", 44153, 34060, 1.5, 1.5, 0, "Machine", "Engineering"},</v>
       </c>
       <c r="O219" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32895,8 +32922,8 @@
         <v>44317 - 34092</v>
       </c>
       <c r="N220" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["44317 - 34092"] +{"Merciless Nether Drake", 44317, 34092, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["44317 - 34092"] ={"Merciless Nether Drake", 44317, 34092, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
       </c>
       <c r="O220" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32939,8 +32966,8 @@
         <v>44744 - 34092</v>
       </c>
       <c r="N221" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["44744 - 34092"] +{"Merciless Nether Drake", 44744, 34092, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["44744 - 34092"] ={"Merciless Nether Drake", 44744, 34092, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
       </c>
       <c r="O221" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -32986,8 +33013,8 @@
         <v>46197 - 35225</v>
       </c>
       <c r="N222" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46197 - 35225"] +{"X-51 Nether-Rocket", 46197, 35225, 1.5, 1.5, 0, "Rocket", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46197 - 35225"] ={"X-51 Nether-Rocket", 46197, 35225, 1.5, 1.5, 0, "Rocket", "Duplicate"},</v>
       </c>
       <c r="O222" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33033,8 +33060,8 @@
         <v>46197 - 49285</v>
       </c>
       <c r="N223" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46197 - 49285"] +{"X-51 Nether-Rocket", 46197, 49285, 1.5, 1.5, 0, "Rocket", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46197 - 49285"] ={"X-51 Nether-Rocket", 46197, 49285, 1.5, 1.5, 0, "Rocket", "Duplicate"},</v>
       </c>
       <c r="O223" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33080,8 +33107,8 @@
         <v>46197 - 198629</v>
       </c>
       <c r="N224" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46197 - 198629"] +{"X-51 Nether-Rocket", 46197, 198629, 1.5, 1.5, 0, "Rocket", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46197 - 198629"] ={"X-51 Nether-Rocket", 46197, 198629, 1.5, 1.5, 0, "Rocket", "TCG"},</v>
       </c>
       <c r="O224" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33127,8 +33154,8 @@
         <v>46199 - 35226</v>
       </c>
       <c r="N225" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46199 - 35226"] +{"X-51 Nether-Rocket X-TREME", 46199, 35226, 2.8, 2.8, 0, "Rocket", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46199 - 35226"] ={"X-51 Nether-Rocket X-TREME", 46199, 35226, 2.8, 2.8, 0, "Rocket", "Duplicate"},</v>
       </c>
       <c r="O225" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33174,8 +33201,8 @@
         <v>46199 - 49286</v>
       </c>
       <c r="N226" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46199 - 49286"] +{"X-51 Nether-Rocket X-TREME", 46199, 49286, 2.8, 2.8, 0, "Rocket", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46199 - 49286"] ={"X-51 Nether-Rocket X-TREME", 46199, 49286, 2.8, 2.8, 0, "Rocket", "Duplicate"},</v>
       </c>
       <c r="O226" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33221,8 +33248,8 @@
         <v>46199 - 198628</v>
       </c>
       <c r="N227" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46199 - 198628"] +{"X-51 Nether-Rocket X-TREME", 46199, 198628, 2.8, 2.8, 0, "Rocket", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46199 - 198628"] ={"X-51 Nether-Rocket X-TREME", 46199, 198628, 2.8, 2.8, 0, "Rocket", "TCG"},</v>
       </c>
       <c r="O227" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33271,8 +33298,8 @@
         <v>46628 - 35513</v>
       </c>
       <c r="N228" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["46628 - 35513"] +{"Swift White Hawkstrider", 46628, 35513, 1, 1, 0, "Hawkstrider", "Drop Magisters' Terrace"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["46628 - 35513"] ={"Swift White Hawkstrider", 46628, 35513, 1, 1, 0, "Hawkstrider", "Drop Magisters' Terrace"},</v>
       </c>
       <c r="O228" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33318,8 +33345,8 @@
         <v>47037 - 0</v>
       </c>
       <c r="N229" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["47037 - 0"] +{"Swift War Elekk", 47037, 0, 1, 1, 0, "Elekk", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["47037 - 0"] ={"Swift War Elekk", 47037, 0, 1, 1, 0, "Elekk", "removed"},</v>
       </c>
       <c r="O229" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33368,8 +33395,8 @@
         <v>48025 - 37012</v>
       </c>
       <c r="N230" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["48025 - 37012"] +{"Headless Horseman's Mount", 48025, 37012, 2.8, 0.6, 0, "Horse", "Drop, Halloween"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["48025 - 37012"] ={"Headless Horseman's Mount", 48025, 37012, 2.8, 0.6, 0, "Horse", "Drop, Halloween"},</v>
       </c>
       <c r="O230" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33415,8 +33442,8 @@
         <v>48027 - 35906</v>
       </c>
       <c r="N231" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["48027 - 35906"] +{"Black War Elekk", 48027, 35906, 1, 1, 0, "Elekk", "Honor"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["48027 - 35906"] ={"Black War Elekk", 48027, 35906, 1, 1, 0, "Elekk", "Honor"},</v>
       </c>
       <c r="O231" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33462,8 +33489,8 @@
         <v>48778 - 0</v>
       </c>
       <c r="N232" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["48778 - 0"] +{"Acherus Deathcharger", 48778, 0, 1, 1, 0, "DeathKnight", "DeathKnight"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["48778 - 0"] ={"Acherus Deathcharger", 48778, 0, 1, 1, 0, "DeathKnight", "DeathKnight"},</v>
       </c>
       <c r="O232" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33509,8 +33536,8 @@
         <v>48954 - 37598</v>
       </c>
       <c r="N233" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["48954 - 37598"] +{"Swift Zhevra", 48954, 37598, 1, 1, 0, "Horse", "Recruit a Friend"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["48954 - 37598"] ={"Swift Zhevra", 48954, 37598, 1, 1, 0, "Horse", "Recruit a Friend"},</v>
       </c>
       <c r="O233" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33556,8 +33583,8 @@
         <v>49193 - 37676</v>
       </c>
       <c r="N234" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["49193 - 37676"] +{"Vengeful Nether Drake", 49193, 37676, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["49193 - 37676"] ={"Vengeful Nether Drake", 49193, 37676, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
       </c>
       <c r="O234" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33603,8 +33630,8 @@
         <v>49322 - 37719</v>
       </c>
       <c r="N235" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["49322 - 37719"] +{"Swift Zhevra", 49322, 37719, 1, 1, 0, "Horse", "Recruit a Friend"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["49322 - 37719"] ={"Swift Zhevra", 49322, 37719, 1, 1, 0, "Horse", "Recruit a Friend"},</v>
       </c>
       <c r="O235" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33650,8 +33677,8 @@
         <v>49378 - 37827</v>
       </c>
       <c r="N236" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["49378 - 37827"] +{"Brewfest Riding Kodo", 49378, 37827, 0.6, 0.6, 0, "Kodo", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["49378 - 37827"] ={"Brewfest Riding Kodo", 49378, 37827, 0.6, 0.6, 0, "Kodo", "Duplicate"},</v>
       </c>
       <c r="O236" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33700,8 +33727,8 @@
         <v>49379 - 37828</v>
       </c>
       <c r="N237" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["49379 - 37828"] +{"Great Brewfest Kodo", 49379, 37828, 1, 1, 0, "Kodo", "Drop Brewfest"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["49379 - 37828"] ={"Great Brewfest Kodo", 49379, 37828, 1, 1, 0, "Kodo", "Drop Brewfest"},</v>
       </c>
       <c r="O237" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33747,8 +33774,8 @@
         <v>50869 - 37827</v>
       </c>
       <c r="N238" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["50869 - 37827"] +{"Brewfest Kodo", 50869, 37827, 0.6, 0.6, 0, "Kodo", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["50869 - 37827"] ={"Brewfest Kodo", 50869, 37827, 0.6, 0.6, 0, "Kodo", "Duplicate"},</v>
       </c>
       <c r="O238" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33794,8 +33821,8 @@
         <v>50870 - 33976</v>
       </c>
       <c r="N239" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["50870 - 33976"] +{"Brewfest Ram", 50870, 33976, 0.6, 0.6, 0, "Ram", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["50870 - 33976"] ={"Brewfest Ram", 50870, 33976, 0.6, 0.6, 0, "Ram", "Duplicate"},</v>
       </c>
       <c r="O239" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33841,8 +33868,8 @@
         <v>51412 - 38576</v>
       </c>
       <c r="N240" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["51412 - 38576"] +{"Big Battle Bear", 51412, 38576, 1, 1, 0, "Bear", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["51412 - 38576"] ={"Big Battle Bear", 51412, 38576, 1, 1, 0, "Bear", "Duplicate"},</v>
       </c>
       <c r="O240" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33888,8 +33915,8 @@
         <v>51412 - 49282</v>
       </c>
       <c r="N241" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["51412 - 49282"] +{"Big Battle Bear", 51412, 49282, 1, 1, 0, "Bear", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["51412 - 49282"] ={"Big Battle Bear", 51412, 49282, 1, 1, 0, "Bear", "Duplicate"},</v>
       </c>
       <c r="O241" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33935,8 +33962,8 @@
         <v>51412 - 198632</v>
       </c>
       <c r="N242" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["51412 - 198632"] +{"Big Battle Bear", 51412, 198632, 1, 1, 0, "Bear", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["51412 - 198632"] ={"Big Battle Bear", 51412, 198632, 1, 1, 0, "Bear", "TCG"},</v>
       </c>
       <c r="O242" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -33982,8 +34009,8 @@
         <v>51960 - 38690</v>
       </c>
       <c r="N243" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["51960 - 38690"] +{"Frost Wyrm Mount", 51960, 38690, 2.8, 2.8, 0, "Wyrm", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["51960 - 38690"] ={"Frost Wyrm Mount", 51960, 38690, 2.8, 2.8, 0, "Wyrm", "Removed"},</v>
       </c>
       <c r="O243" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34029,8 +34056,8 @@
         <v>54729 - 40775</v>
       </c>
       <c r="N244" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["54729 - 40775"] +{"Winged Steed of the Ebon Blade", 54729, 40775, 2.8, 2.8, 0, "Wyrm", "DeathKnight"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["54729 - 40775"] ={"Winged Steed of the Ebon Blade", 54729, 40775, 2.8, 2.8, 0, "Wyrm", "DeathKnight"},</v>
       </c>
       <c r="O244" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34070,8 +34097,8 @@
         <v>54753 - 40777</v>
       </c>
       <c r="N245" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["54753 - 40777"] +{"White Polar Bear", 54753, 40777, 1, 1, 0, "Bear", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["54753 - 40777"] ={"White Polar Bear", 54753, 40777, 1, 1, 0, "Bear", "Duplicate"},</v>
       </c>
       <c r="O245" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34120,8 +34147,8 @@
         <v>54753 - 43962</v>
       </c>
       <c r="N246" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["54753 - 43962"] +{"White Polar Bear", 54753, 43962, 1, 1, 0, "Bear", "Daily Storm Peaks"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["54753 - 43962"] ={"White Polar Bear", 54753, 43962, 1, 1, 0, "Bear", "Daily Storm Peaks"},</v>
       </c>
       <c r="O246" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34164,8 +34191,8 @@
         <v>55531 - 41508</v>
       </c>
       <c r="N247" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["55531 - 41508"] +{"Mechano-hog", 55531, 41508, 1, 1, 0, "Machine", "Engineering"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["55531 - 41508"] ={"Mechano-hog", 55531, 41508, 1, 1, 0, "Machine", "Engineering"},</v>
       </c>
       <c r="O247" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34211,8 +34238,8 @@
         <v>58615 - 43516</v>
       </c>
       <c r="N248" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["58615 - 43516"] +{"Brutal Nether Drake", 58615, 43516, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["58615 - 43516"] ={"Brutal Nether Drake", 58615, 43516, 3.1, 3.1, 0, "Nether Drake", "Gladiator"},</v>
       </c>
       <c r="O248" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34258,8 +34285,8 @@
         <v>58983 - 43599</v>
       </c>
       <c r="N249" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["58983 - 43599"] +{"Big Blizzard Bear", 58983, 43599, 1, 1, 0, "Bear", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["58983 - 43599"] ={"Big Blizzard Bear", 58983, 43599, 1, 1, 0, "Bear", "TCG"},</v>
       </c>
       <c r="O249" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34308,8 +34335,8 @@
         <v>59567 - 43952</v>
       </c>
       <c r="N250" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59567 - 43952"] +{"Azure Drake", 59567, 43952, 2.8, 2.8, 0, "Drake", "Drop Eye of Eternity"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59567 - 43952"] ={"Azure Drake", 59567, 43952, 2.8, 2.8, 0, "Drake", "Drop Eye of Eternity"},</v>
       </c>
       <c r="O250" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34358,8 +34385,8 @@
         <v>59568 - 43953</v>
       </c>
       <c r="N251" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59568 - 43953"] +{"Blue Drake", 59568, 43953, 2.8, 2.8, 0, "Drake", "Drop, The Eye of Eternity"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59568 - 43953"] ={"Blue Drake", 59568, 43953, 2.8, 2.8, 0, "Drake", "Drop, The Eye of Eternity"},</v>
       </c>
       <c r="O251" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34408,8 +34435,8 @@
         <v>59569 - 43951</v>
       </c>
       <c r="N252" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59569 - 43951"] +{"Bronze Drake", 59569, 43951, 2.8, 2.8, 0, "Drake", "Drop The Culling of Stratholme"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59569 - 43951"] ={"Bronze Drake", 59569, 43951, 2.8, 2.8, 0, "Drake", "Drop The Culling of Stratholme"},</v>
       </c>
       <c r="O252" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34458,8 +34485,8 @@
         <v>59570 - 43955</v>
       </c>
       <c r="N253" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59570 - 43955"] +{"Red Drake", 59570, 43955, 2.8, 2.8, 0, "Drake", "Exalted, Wyrmrest Accord"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59570 - 43955"] ={"Red Drake", 59570, 43955, 2.8, 2.8, 0, "Drake", "Exalted, Wyrmrest Accord"},</v>
       </c>
       <c r="O253" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34508,8 +34535,8 @@
         <v>59571 - 43954</v>
       </c>
       <c r="N254" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59571 - 43954"] +{"Twilight Drake", 59571, 43954, 2.8, 2.8, 0, "Drake", "Drop, The Obsidian Sanctum"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59571 - 43954"] ={"Twilight Drake", 59571, 43954, 2.8, 2.8, 0, "Drake", "Drop, The Obsidian Sanctum"},</v>
       </c>
       <c r="O254" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34555,8 +34582,8 @@
         <v>59572 - 43964</v>
       </c>
       <c r="N255" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59572 - 43964"] +{"Black Polar Bear", 59572, 43964, 1, 1, 0, "Bear", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59572 - 43964"] ={"Black Polar Bear", 59572, 43964, 1, 1, 0, "Bear", "Removed"},</v>
       </c>
       <c r="O255" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34602,8 +34629,8 @@
         <v>59573 - 43963</v>
       </c>
       <c r="N256" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59573 - 43963"] +{"Brown Polar Bear", 59573, 43963, 1, 1, 0, "Bear", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59573 - 43963"] ={"Brown Polar Bear", 59573, 43963, 1, 1, 0, "Bear", "Removed"},</v>
       </c>
       <c r="O256" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34652,8 +34679,8 @@
         <v>59650 - 43986</v>
       </c>
       <c r="N257" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59650 - 43986"] +{"Black Drake", 59650, 43986, 2.8, 2.8, 0, "Drake", "Drop, The Obsidian Sanctum"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59650 - 43986"] ={"Black Drake", 59650, 43986, 2.8, 2.8, 0, "Drake", "Drop, The Obsidian Sanctum"},</v>
       </c>
       <c r="O257" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34699,8 +34726,8 @@
         <v>59785 - 43956</v>
       </c>
       <c r="N258" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59785 - 43956"] +{"Black War Mammoth", 59785, 43956, 1, 1, 0, "Mammoth", "Stone Keeper's Shard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59785 - 43956"] ={"Black War Mammoth", 59785, 43956, 1, 1, 0, "Mammoth", "Stone Keeper's Shard"},</v>
       </c>
       <c r="O258" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34743,8 +34770,8 @@
         <v>59788 - 44077</v>
       </c>
       <c r="N259" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59788 - 44077"] +{"Black War Mammoth", 59788, 44077, 1, 1, 0, "Mammoth", "Stone Keeper's Shard"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59788 - 44077"] ={"Black War Mammoth", 59788, 44077, 1, 1, 0, "Mammoth", "Stone Keeper's Shard"},</v>
       </c>
       <c r="O259" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34790,8 +34817,8 @@
         <v>59791 - 44230</v>
       </c>
       <c r="N260" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59791 - 44230"] +{"Wooly Mammoth", 59791, 44230, 1, 1, 0, "Mammoth", "Embelm of Heroism"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59791 - 44230"] ={"Wooly Mammoth", 59791, 44230, 1, 1, 0, "Mammoth", "Embelm of Heroism"},</v>
       </c>
       <c r="O260" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34834,8 +34861,8 @@
         <v>59793 - 44231</v>
       </c>
       <c r="N261" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59793 - 44231"] +{"Wooly Mammoth", 59793, 44231, 1, 1, 0, "Mammoth", "Embelm of Heroism"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59793 - 44231"] ={"Wooly Mammoth", 59793, 44231, 1, 1, 0, "Mammoth", "Embelm of Heroism"},</v>
       </c>
       <c r="O261" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34881,8 +34908,8 @@
         <v>59797 - 43958</v>
       </c>
       <c r="N262" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59797 - 43958"] +{"Ice Mammoth", 59797, 43958, 1, 1, 0, "Mammoth", "Revered Sons of Hodir"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59797 - 43958"] ={"Ice Mammoth", 59797, 43958, 1, 1, 0, "Mammoth", "Revered Sons of Hodir"},</v>
       </c>
       <c r="O262" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34925,8 +34952,8 @@
         <v>59799 - 44080</v>
       </c>
       <c r="N263" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59799 - 44080"] +{"Ice Mammoth", 59799, 44080, 1, 1, 0, "Mammoth", "Revered Sons of Hodir"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59799 - 44080"] ={"Ice Mammoth", 59799, 44080, 1, 1, 0, "Mammoth", "Revered Sons of Hodir"},</v>
       </c>
       <c r="O263" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -34972,8 +34999,8 @@
         <v>59802 - 43961</v>
       </c>
       <c r="N264" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59802 - 43961"] +{"Grand Ice Mammoth", 59802, 43961, 1, 1, 0, "Mammoth", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59802 - 43961"] ={"Grand Ice Mammoth", 59802, 43961, 1, 1, 0, "Mammoth", "Removed"},</v>
       </c>
       <c r="O264" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35019,8 +35046,8 @@
         <v>59804 - 44086</v>
       </c>
       <c r="N265" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59804 - 44086"] +{"Grand Ice Mammoth", 59804, 44086, 1, 1, 0, "Mammoth", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59804 - 44086"] ={"Grand Ice Mammoth", 59804, 44086, 1, 1, 0, "Mammoth", "Removed"},</v>
       </c>
       <c r="O265" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35069,8 +35096,8 @@
         <v>59961 - 44160</v>
       </c>
       <c r="N266" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59961 - 44160"] +{"Red Proto-Drake", 59961, 44160, 2.8, 2.8, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59961 - 44160"] ={"Red Proto-Drake", 59961, 44160, 2.8, 2.8, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O266" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35119,8 +35146,8 @@
         <v>59976 - 44164</v>
       </c>
       <c r="N267" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59976 - 44164"] +{"Black Proto-Drake", 59976, 44164, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59976 - 44164"] ={"Black Proto-Drake", 59976, 44164, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O267" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35169,8 +35196,8 @@
         <v>59996 - 44151</v>
       </c>
       <c r="N268" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["59996 - 44151"] +{"Blue Proto-Drake", 59996, 44151, 2.8, 2.8, 0, "Proto-Drake", "Drop, Skadi the Ruthless"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["59996 - 44151"] ={"Blue Proto-Drake", 59996, 44151, 2.8, 2.8, 0, "Proto-Drake", "Drop, Skadi the Ruthless"},</v>
       </c>
       <c r="O268" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35219,8 +35246,8 @@
         <v>60002 - 44168</v>
       </c>
       <c r="N269" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60002 - 44168"] +{"Time-Lost Proto-Drake", 60002, 44168, 2.8, 2.8, 0, "Proto-Drake", "Drop Rare"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60002 - 44168"] ={"Time-Lost Proto-Drake", 60002, 44168, 2.8, 2.8, 0, "Proto-Drake", "Drop Rare"},</v>
       </c>
       <c r="O269" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35269,8 +35296,8 @@
         <v>60021 - 44175</v>
       </c>
       <c r="N270" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60021 - 44175"] +{"Plagued Proto-Drake", 60021, 44175, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60021 - 44175"] ={"Plagued Proto-Drake", 60021, 44175, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O270" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35319,8 +35346,8 @@
         <v>60024 - 44177</v>
       </c>
       <c r="N271" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60024 - 44177"] +{"Violet Proto-Drake", 60024, 44177, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60024 - 44177"] ={"Violet Proto-Drake", 60024, 44177, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O271" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35369,8 +35396,8 @@
         <v>60025 - 44178</v>
       </c>
       <c r="N272" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60025 - 44178"] +{"Albino Drake", 60025, 44178, 2.8, 2.8, 0, "Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60025 - 44178"] ={"Albino Drake", 60025, 44178, 2.8, 2.8, 0, "Drake", "Achievment"},</v>
       </c>
       <c r="O272" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35416,8 +35443,8 @@
         <v>60114 - 44225</v>
       </c>
       <c r="N273" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60114 - 44225"] +{"Armored Brown Bear", 60114, 44225, 1, 1, 0, "Bear", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60114 - 44225"] ={"Armored Brown Bear", 60114, 44225, 1, 1, 0, "Bear", "Gold"},</v>
       </c>
       <c r="O273" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35460,8 +35487,8 @@
         <v>60116 - 44226</v>
       </c>
       <c r="N274" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60116 - 44226"] +{"Armored Brown Bear", 60116, 44226, 1, 1, 0, "Bear", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60116 - 44226"] ={"Armored Brown Bear", 60116, 44226, 1, 1, 0, "Bear", "Gold"},</v>
       </c>
       <c r="O274" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35507,8 +35534,8 @@
         <v>60118 - 44223</v>
       </c>
       <c r="N275" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60118 - 44223"] +{"Black War Bear", 60118, 44223, 1, 1, 0, "Bear", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60118 - 44223"] ={"Black War Bear", 60118, 44223, 1, 1, 0, "Bear", "Achievment"},</v>
       </c>
       <c r="O275" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35551,8 +35578,8 @@
         <v>60119 - 44224</v>
       </c>
       <c r="N276" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60119 - 44224"] +{"Black War Bear", 60119, 44224, 1, 1, 0, "Bear", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60119 - 44224"] ={"Black War Bear", 60119, 44224, 1, 1, 0, "Bear", "Achievment"},</v>
       </c>
       <c r="O276" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35598,8 +35625,8 @@
         <v>60136 - 0</v>
       </c>
       <c r="N277" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60136 - 0"] +{"Grand Caravan Mammoth", 60136, 0, 1, 1, 0, "Mammoth", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60136 - 0"] ={"Grand Caravan Mammoth", 60136, 0, 1, 1, 0, "Mammoth", "removed"},</v>
       </c>
       <c r="O277" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35645,8 +35672,8 @@
         <v>60140 - 0</v>
       </c>
       <c r="N278" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60140 - 0"] +{"Grand Caravan Mammoth", 60140, 0, 1, 1, 0, "Mammoth", "removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60140 - 0"] ={"Grand Caravan Mammoth", 60140, 0, 1, 1, 0, "Mammoth", "removed"},</v>
       </c>
       <c r="O278" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35692,8 +35719,8 @@
         <v>60424 - 44413</v>
       </c>
       <c r="N279" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["60424 - 44413"] +{"Mekgineer's Chopper", 60424, 44413, 1, 1, 0, "Machine", "Engineering"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["60424 - 44413"] ={"Mekgineer's Chopper", 60424, 44413, 1, 1, 0, "Machine", "Engineering"},</v>
       </c>
       <c r="O279" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35739,8 +35766,8 @@
         <v>61229 - 44689</v>
       </c>
       <c r="N280" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61229 - 44689"] +{"Armored Snowy Gryphon", 61229, 44689, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61229 - 44689"] ={"Armored Snowy Gryphon", 61229, 44689, 2.8, 2.8, 0, "Gryphon", "Gold"},</v>
       </c>
       <c r="O280" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35783,8 +35810,8 @@
         <v>61230 - 44690</v>
       </c>
       <c r="N281" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61230 - 44690"] +{"Armored Blue Wind Rider", 61230, 44690, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61230 - 44690"] ={"Armored Blue Wind Rider", 61230, 44690, 2.8, 2.8, 0, "Wind Rider", "Gold"},</v>
       </c>
       <c r="O281" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35833,8 +35860,8 @@
         <v>61294 - 44707</v>
       </c>
       <c r="N282" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61294 - 44707"] +{"Green Proto-Drake", 61294, 44707, 2.8, 2.8, 0, "Proto-Drake", "Revered Oracles, Mysterious Egg"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61294 - 44707"] ={"Green Proto-Drake", 61294, 44707, 2.8, 2.8, 0, "Proto-Drake", "Revered Oracles, Mysterious Egg"},</v>
       </c>
       <c r="O282" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35880,8 +35907,8 @@
         <v>61309 - 44558</v>
       </c>
       <c r="N283" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61309 - 44558"] +{"Magnificent Flying Carpet", 61309, 44558, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61309 - 44558"] ={"Magnificent Flying Carpet", 61309, 44558, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O283" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35924,8 +35951,8 @@
         <v>61425 - 44234</v>
       </c>
       <c r="N284" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61425 - 44234"] +{"Traveler's Tundra Mammoth", 61425, 44234, 1, 1, 0, "Mammoth", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61425 - 44234"] ={"Traveler's Tundra Mammoth", 61425, 44234, 1, 1, 0, "Mammoth", "Gold"},</v>
       </c>
       <c r="O284" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -35971,8 +35998,8 @@
         <v>61442 - 44555</v>
       </c>
       <c r="N285" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61442 - 44555"] +{"Swift Mooncloth Carpet", 61442, 44555, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61442 - 44555"] ={"Swift Mooncloth Carpet", 61442, 44555, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O285" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36018,8 +36045,8 @@
         <v>61444 - 44557</v>
       </c>
       <c r="N286" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61444 - 44557"] +{"Swift Shadoweave Carpet", 61444, 44557, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61444 - 44557"] ={"Swift Shadoweave Carpet", 61444, 44557, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O286" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36065,8 +36092,8 @@
         <v>61446 - 44556</v>
       </c>
       <c r="N287" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61446 - 44556"] +{"Swift Spellfire Carpet", 61446, 44556, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61446 - 44556"] ={"Swift Spellfire Carpet", 61446, 44556, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O287" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36112,8 +36139,8 @@
         <v>61447 - 44235</v>
       </c>
       <c r="N288" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61447 - 44235"] +{"Traveler's Tundra Mammoth", 61447, 44235, 1, 1, 0, "Mammoth", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61447 - 44235"] ={"Traveler's Tundra Mammoth", 61447, 44235, 1, 1, 0, "Mammoth", "Gold"},</v>
       </c>
       <c r="O288" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36159,8 +36186,8 @@
         <v>61451 - 44554</v>
       </c>
       <c r="N289" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61451 - 44554"] +{"Flying Carpet", 61451, 44554, 1.5, 1.5, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61451 - 44554"] ={"Flying Carpet", 61451, 44554, 1.5, 1.5, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O289" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36206,8 +36233,8 @@
         <v>61465 - 43959</v>
       </c>
       <c r="N290" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61465 - 43959"] +{"Grand Black War Mammoth", 61465, 43959, 1, 1, 0, "Mammoth", "Drop Vault"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61465 - 43959"] ={"Grand Black War Mammoth", 61465, 43959, 1, 1, 0, "Mammoth", "Drop Vault"},</v>
       </c>
       <c r="O290" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36250,8 +36277,8 @@
         <v>61467 - 44083</v>
       </c>
       <c r="N291" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61467 - 44083"] +{"Grand Black War Mammoth", 61467, 44083, 1, 1, 0, "Mammoth", "Drop Vault"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61467 - 44083"] ={"Grand Black War Mammoth", 61467, 44083, 1, 1, 0, "Mammoth", "Drop Vault"},</v>
       </c>
       <c r="O291" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36297,8 +36324,8 @@
         <v>61469 - 43961</v>
       </c>
       <c r="N292" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61469 - 43961"] +{"Grand Ice Mammoth", 61469, 43961, 1, 1, 0, "Mammoth", "Exaulted Sons of Hodir"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61469 - 43961"] ={"Grand Ice Mammoth", 61469, 43961, 1, 1, 0, "Mammoth", "Exaulted Sons of Hodir"},</v>
       </c>
       <c r="O292" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36341,8 +36368,8 @@
         <v>61470 - 44086</v>
       </c>
       <c r="N293" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61470 - 44086"] +{"Grand Ice Mammoth", 61470, 44086, 1, 1, 0, "Mammoth", "Exaulted Sons of Hodir"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61470 - 44086"] ={"Grand Ice Mammoth", 61470, 44086, 1, 1, 0, "Mammoth", "Exaulted Sons of Hodir"},</v>
       </c>
       <c r="O293" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36388,8 +36415,8 @@
         <v>61996 - 44843</v>
       </c>
       <c r="N294" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61996 - 44843"] +{"Blue Dragonhawk", 61996, 44843, 2.8, 2.8, 0, "DragonHawk", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61996 - 44843"] ={"Blue Dragonhawk", 61996, 44843, 2.8, 2.8, 0, "DragonHawk", "Achievment"},</v>
       </c>
       <c r="O294" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36432,8 +36459,8 @@
         <v>61997 - 44842</v>
       </c>
       <c r="N295" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["61997 - 44842"] +{"Red Dragonhawk", 61997, 44842, 2.8, 2.8, 0, "DragonHawk", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["61997 - 44842"] ={"Red Dragonhawk", 61997, 44842, 2.8, 2.8, 0, "DragonHawk", "Achievment"},</v>
       </c>
       <c r="O295" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36479,8 +36506,8 @@
         <v>62048 - 44857</v>
       </c>
       <c r="N296" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["62048 - 44857"] +{"Black Dragonhawk Mount", 62048, 44857, 2.8, 2.8, 0, "DragonHawk", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["62048 - 44857"] ={"Black Dragonhawk Mount", 62048, 44857, 2.8, 2.8, 0, "DragonHawk", "Removed"},</v>
       </c>
       <c r="O296" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36526,8 +36553,8 @@
         <v>63232 - 45125</v>
       </c>
       <c r="N297" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63232 - 45125"] +{"Stormwind Steed", 63232, 45125, 1, 1, 0, "Horse", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63232 - 45125"] ={"Stormwind Steed", 63232, 45125, 1, 1, 0, "Horse", "Champion's Seals"},</v>
       </c>
       <c r="O297" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36570,8 +36597,8 @@
         <v>63635 - 45593</v>
       </c>
       <c r="N298" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63635 - 45593"] +{"Darkspear Raptor", 63635, 45593, 1, 1, 0, "Raptor", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63635 - 45593"] ={"Darkspear Raptor", 63635, 45593, 1, 1, 0, "Raptor", "Removed"},</v>
       </c>
       <c r="O298" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36617,8 +36644,8 @@
         <v>63636 - 45586</v>
       </c>
       <c r="N299" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63636 - 45586"] +{"Ironforge Ram", 63636, 45586, 1, 1, 0, "Ram", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63636 - 45586"] ={"Ironforge Ram", 63636, 45586, 1, 1, 0, "Ram", "Champion's Seals"},</v>
       </c>
       <c r="O299" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36664,8 +36691,8 @@
         <v>63637 - 45591</v>
       </c>
       <c r="N300" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63637 - 45591"] +{"Darnassian Nightsaber", 63637, 45591, 1, 1, 0, "Saber", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63637 - 45591"] ={"Darnassian Nightsaber", 63637, 45591, 1, 1, 0, "Saber", "Champion's Seals"},</v>
       </c>
       <c r="O300" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36711,8 +36738,8 @@
         <v>63638 - 45589</v>
       </c>
       <c r="N301" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63638 - 45589"] +{"Gnomeregan Mechanostrider", 63638, 45589, 1, 1, 0, "Mechanostrider", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63638 - 45589"] ={"Gnomeregan Mechanostrider", 63638, 45589, 1, 1, 0, "Mechanostrider", "Champion's Seals"},</v>
       </c>
       <c r="O301" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36758,8 +36785,8 @@
         <v>63639 - 45590</v>
       </c>
       <c r="N302" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63639 - 45590"] +{"Exodar Elekk", 63639, 45590, 1, 1, 0, "Elekk", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63639 - 45590"] ={"Exodar Elekk", 63639, 45590, 1, 1, 0, "Elekk", "Champion's Seals"},</v>
       </c>
       <c r="O302" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36802,8 +36829,8 @@
         <v>63640 - 45595</v>
       </c>
       <c r="N303" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63640 - 45595"] +{"Orgrimmar Wolf", 63640, 45595, 1, 1, 0, "Wolf", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63640 - 45595"] ={"Orgrimmar Wolf", 63640, 45595, 1, 1, 0, "Wolf", "Champion's Seals"},</v>
       </c>
       <c r="O303" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36846,8 +36873,8 @@
         <v>63641 - 45592</v>
       </c>
       <c r="N304" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63641 - 45592"] +{"Thunder Bluff Kodo", 63641, 45592, 1, 1, 0, "Kodo", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63641 - 45592"] ={"Thunder Bluff Kodo", 63641, 45592, 1, 1, 0, "Kodo", "Champion's Seals"},</v>
       </c>
       <c r="O304" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36890,8 +36917,8 @@
         <v>63642 - 45596</v>
       </c>
       <c r="N305" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63642 - 45596"] +{"Silvermoon Hawkstrider", 63642, 45596, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63642 - 45596"] ={"Silvermoon Hawkstrider", 63642, 45596, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
       </c>
       <c r="O305" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36934,8 +36961,8 @@
         <v>63643 - 45597</v>
       </c>
       <c r="N306" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63643 - 45597"] +{"Forsaken Warhorse", 63643, 45597, 1, 1, 0, "Horse", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63643 - 45597"] ={"Forsaken Warhorse", 63643, 45597, 1, 1, 0, "Horse", "Champion's Seals"},</v>
       </c>
       <c r="O306" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -36984,8 +37011,8 @@
         <v>63796 - 45693</v>
       </c>
       <c r="N307" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63796 - 45693"] +{"Mimiron's Head", 63796, 45693, 3.1, 3.1, 0, "Machine", "Drop Ulduar"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63796 - 45693"] ={"Mimiron's Head", 63796, 45693, 3.1, 3.1, 0, "Machine", "Drop Ulduar"},</v>
       </c>
       <c r="O307" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37034,8 +37061,8 @@
         <v>63844 - 45725</v>
       </c>
       <c r="N308" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63844 - 45725"] +{"Argent Hippogryph", 63844, 45725, 2.8, 2.8, 0, "Hippogryph", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63844 - 45725"] ={"Argent Hippogryph", 63844, 45725, 2.8, 2.8, 0, "Hippogryph", "Champion's Seals"},</v>
       </c>
       <c r="O308" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37084,8 +37111,8 @@
         <v>63956 - 45801</v>
       </c>
       <c r="N309" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63956 - 45801"] +{"Ironbound Proto-Drake", 63956, 45801, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63956 - 45801"] ={"Ironbound Proto-Drake", 63956, 45801, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O309" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37134,8 +37161,8 @@
         <v>63963 - 45802</v>
       </c>
       <c r="N310" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["63963 - 45802"] +{"Rusted Proto-Drake", 63963, 45802, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["63963 - 45802"] ={"Rusted Proto-Drake", 63963, 45802, 3.1, 3.1, 0, "Proto-Drake", "Achievment"},</v>
       </c>
       <c r="O310" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37178,8 +37205,8 @@
         <v>64656 - 46101</v>
       </c>
       <c r="N311" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64656 - 46101"] +{"Blue Skeletal Warhorse", 64656, 46101, 1, 1, 0, "Horse", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64656 - 46101"] ={"Blue Skeletal Warhorse", 64656, 46101, 1, 1, 0, "Horse", "Removed"},</v>
       </c>
       <c r="O311" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37222,8 +37249,8 @@
         <v>64657 - 46100</v>
       </c>
       <c r="N312" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64657 - 46100"] +{"White Kodo", 64657, 46100, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64657 - 46100"] ={"White Kodo", 64657, 46100, 0.6, 0.6, 0, "Kodo", "Gold"},</v>
       </c>
       <c r="O312" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37266,8 +37293,8 @@
         <v>64658 - 46099</v>
       </c>
       <c r="N313" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64658 - 46099"] +{"Black Wolf", 64658, 46099, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64658 - 46099"] ={"Black Wolf", 64658, 46099, 0.6, 0.6, 0, "Wolf", "Gold"},</v>
       </c>
       <c r="O313" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37310,8 +37337,8 @@
         <v>64659 - 46102</v>
       </c>
       <c r="N314" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64659 - 46102"] +{"Venomhide Ravasaur", 64659, 46102, 1, 1, 0, "Raptor", "Dailies Ungoro Crator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64659 - 46102"] ={"Venomhide Ravasaur", 64659, 46102, 1, 1, 0, "Raptor", "Dailies Ungoro Crator"},</v>
       </c>
       <c r="O314" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37360,8 +37387,8 @@
         <v>64731 - 46109</v>
       </c>
       <c r="N315" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64731 - 46109"] +{"Sea Turtle", 64731, 46109, 0, 0, 1, "Turtle", "fishing"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64731 - 46109"] ={"Sea Turtle", 64731, 46109, 0, 0, 1, "Turtle", "fishing"},</v>
       </c>
       <c r="O315" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37407,8 +37434,8 @@
         <v>64927 - 46708</v>
       </c>
       <c r="N316" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64927 - 46708"] +{"Deadly Gladiator's Frost Wyrm", 64927, 46708, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64927 - 46708"] ={"Deadly Gladiator's Frost Wyrm", 64927, 46708, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
       </c>
       <c r="O316" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37451,8 +37478,8 @@
         <v>64977 - 46308</v>
       </c>
       <c r="N317" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["64977 - 46308"] +{"Black Skeletal Horse", 64977, 46308, 0.6, 0.6, 0, "DeadHorse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["64977 - 46308"] ={"Black Skeletal Horse", 64977, 46308, 0.6, 0.6, 0, "DeadHorse", "Gold"},</v>
       </c>
       <c r="O317" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37498,8 +37525,8 @@
         <v>65439 - 46171</v>
       </c>
       <c r="N318" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65439 - 46171"] +{"Furious Gladiator's Frost Wyrm", 65439, 46171, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65439 - 46171"] ={"Furious Gladiator's Frost Wyrm", 65439, 46171, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
       </c>
       <c r="O318" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37542,8 +37569,8 @@
         <v>65637 - 46745</v>
       </c>
       <c r="N319" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65637 - 46745"] +{"Great Red Elekk", 65637, 46745, 1, 1, 0, "Elekk", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65637 - 46745"] ={"Great Red Elekk", 65637, 46745, 1, 1, 0, "Elekk", "Duplicate"},</v>
       </c>
       <c r="O319" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37589,8 +37616,8 @@
         <v>65637 - 46756</v>
       </c>
       <c r="N320" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65637 - 46756"] +{"Great Red Elekk", 65637, 46756, 1, 1, 0, "Elekk", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65637 - 46756"] ={"Great Red Elekk", 65637, 46756, 1, 1, 0, "Elekk", "Champion's Seals"},</v>
       </c>
       <c r="O320" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37636,8 +37663,8 @@
         <v>65638 - 46744</v>
       </c>
       <c r="N321" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65638 - 46744"] +{"Swift Moonsaber", 65638, 46744, 1, 1, 0, "Saber", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65638 - 46744"] ={"Swift Moonsaber", 65638, 46744, 1, 1, 0, "Saber", "Champion's Seals"},</v>
       </c>
       <c r="O321" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37680,8 +37707,8 @@
         <v>65638 - 46759</v>
       </c>
       <c r="N322" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65638 - 46759"] +{"Swift Moonsaber", 65638, 46759, 1, 1, 0, "Saber", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65638 - 46759"] ={"Swift Moonsaber", 65638, 46759, 1, 1, 0, "Saber", "Duplicate"},</v>
       </c>
       <c r="O322" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37724,8 +37751,8 @@
         <v>65639 - 46751</v>
       </c>
       <c r="N323" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65639 - 46751"] +{"Swift Red Hawkstrider", 65639, 46751, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65639 - 46751"] ={"Swift Red Hawkstrider", 65639, 46751, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
       </c>
       <c r="O323" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37768,8 +37795,8 @@
         <v>65639 - 46761</v>
       </c>
       <c r="N324" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65639 - 46761"] +{"Swift Red Hawkstrider", 65639, 46761, 1, 1, 0, "Hawkstrider", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65639 - 46761"] ={"Swift Red Hawkstrider", 65639, 46761, 1, 1, 0, "Hawkstrider", "Duplicate"},</v>
       </c>
       <c r="O324" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37815,8 +37842,8 @@
         <v>65640 - 46752</v>
       </c>
       <c r="N325" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65640 - 46752"] +{"Swift Gray Steed", 65640, 46752, 1, 1, 0, "Horse", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65640 - 46752"] ={"Swift Gray Steed", 65640, 46752, 1, 1, 0, "Horse", "Champion's Seals"},</v>
       </c>
       <c r="O325" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37859,8 +37886,8 @@
         <v>65640 - 46758</v>
       </c>
       <c r="N326" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65640 - 46758"] +{"Swift Gray Steed", 65640, 46758, 1, 1, 0, "Horse", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65640 - 46758"] ={"Swift Gray Steed", 65640, 46758, 1, 1, 0, "Horse", "Duplicate"},</v>
       </c>
       <c r="O326" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37903,8 +37930,8 @@
         <v>65641 - 46750</v>
       </c>
       <c r="N327" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65641 - 46750"] +{"Great Golden Kodo", 65641, 46750, 1, 1, 0, "Kodo", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65641 - 46750"] ={"Great Golden Kodo", 65641, 46750, 1, 1, 0, "Kodo", "Duplicate"},</v>
       </c>
       <c r="O327" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37947,8 +37974,8 @@
         <v>65641 - 46755</v>
       </c>
       <c r="N328" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65641 - 46755"] +{"Great Golden Kodo", 65641, 46755, 1, 1, 0, "Kodo", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65641 - 46755"] ={"Great Golden Kodo", 65641, 46755, 1, 1, 0, "Kodo", "Champion's Seals"},</v>
       </c>
       <c r="O328" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -37994,8 +38021,8 @@
         <v>65642 - 46747</v>
       </c>
       <c r="N329" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65642 - 46747"] +{"Turbostrider", 65642, 46747, 1, 1, 0, "Mechanostrider", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65642 - 46747"] ={"Turbostrider", 65642, 46747, 1, 1, 0, "Mechanostrider", "Champion's Seals"},</v>
       </c>
       <c r="O329" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38038,8 +38065,8 @@
         <v>65642 - 46763</v>
       </c>
       <c r="N330" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65642 - 46763"] +{"Turbostrider", 65642, 46763, 1, 1, 0, "Mechanostrider", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65642 - 46763"] ={"Turbostrider", 65642, 46763, 1, 1, 0, "Mechanostrider", "Duplicate"},</v>
       </c>
       <c r="O330" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38085,8 +38112,8 @@
         <v>65643 - 46748</v>
       </c>
       <c r="N331" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65643 - 46748"] +{"Swift Violet Ram", 65643, 46748, 1, 1, 0, "Ram", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65643 - 46748"] ={"Swift Violet Ram", 65643, 46748, 1, 1, 0, "Ram", "Champion's Seals"},</v>
       </c>
       <c r="O331" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38129,8 +38156,8 @@
         <v>65643 - 46762</v>
       </c>
       <c r="N332" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65643 - 46762"] +{"Swift Violet Ram", 65643, 46762, 1, 1, 0, "Ram", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65643 - 46762"] ={"Swift Violet Ram", 65643, 46762, 1, 1, 0, "Ram", "Duplicate"},</v>
       </c>
       <c r="O332" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38173,8 +38200,8 @@
         <v>65644 - 46743</v>
       </c>
       <c r="N333" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65644 - 46743"] +{"Swift Purple Raptor", 65644, 46743, 1, 1, 0, "Raptor", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65644 - 46743"] ={"Swift Purple Raptor", 65644, 46743, 1, 1, 0, "Raptor", "Champion's Seals"},</v>
       </c>
       <c r="O333" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38217,8 +38244,8 @@
         <v>65644 - 46760</v>
       </c>
       <c r="N334" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65644 - 46760"] +{"Swift Purple Raptor", 65644, 46760, 1, 1, 0, "Raptor", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65644 - 46760"] ={"Swift Purple Raptor", 65644, 46760, 1, 1, 0, "Raptor", "Duplicate"},</v>
       </c>
       <c r="O334" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38261,8 +38288,8 @@
         <v>65645 - 46746</v>
       </c>
       <c r="N335" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65645 - 46746"] +{"White Skeletal Warhorse", 65645, 46746, 1, 1, 0, "Horse", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65645 - 46746"] ={"White Skeletal Warhorse", 65645, 46746, 1, 1, 0, "Horse", "Duplicate"},</v>
       </c>
       <c r="O335" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38305,8 +38332,8 @@
         <v>65645 - 46764</v>
       </c>
       <c r="N336" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65645 - 46764"] +{"White Skeletal Warhorse", 65645, 46764, 1, 1, 0, "Horse", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65645 - 46764"] ={"White Skeletal Warhorse", 65645, 46764, 1, 1, 0, "Horse", "Champion's Seals"},</v>
       </c>
       <c r="O336" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38349,8 +38376,8 @@
         <v>65646 - 46749</v>
       </c>
       <c r="N337" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65646 - 46749"] +{"Swift Burgundy Wolf", 65646, 46749, 1, 1, 0, "Wolf", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65646 - 46749"] ={"Swift Burgundy Wolf", 65646, 46749, 1, 1, 0, "Wolf", "Duplicate"},</v>
       </c>
       <c r="O337" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38393,8 +38420,8 @@
         <v>65646 - 46757</v>
       </c>
       <c r="N338" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["65646 - 46757"] +{"Swift Burgundy Wolf", 65646, 46757, 1, 1, 0, "Wolf", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["65646 - 46757"] ={"Swift Burgundy Wolf", 65646, 46757, 1, 1, 0, "Wolf", "Champion's Seals"},</v>
       </c>
       <c r="O338" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38440,8 +38467,8 @@
         <v>66087 - 46813</v>
       </c>
       <c r="N339" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66087 - 46813"] +{"Silver Covenant Hippogryph", 66087, 46813, 2.8, 2.8, 0, "Hippogryph", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66087 - 46813"] ={"Silver Covenant Hippogryph", 66087, 46813, 2.8, 2.8, 0, "Hippogryph", "Champion's Seals"},</v>
       </c>
       <c r="O339" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38484,8 +38511,8 @@
         <v>66088 - 46814</v>
       </c>
       <c r="N340" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66088 - 46814"] +{"Sunreaver Dragonhawk", 66088, 46814, 2.8, 2.8, 0, "DragonHawk", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66088 - 46814"] ={"Sunreaver Dragonhawk", 66088, 46814, 2.8, 2.8, 0, "DragonHawk", "Champion's Seals"},</v>
       </c>
       <c r="O340" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38534,8 +38561,8 @@
         <v>66090 - 46815</v>
       </c>
       <c r="N341" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66090 - 46815"] +{"Quel'dorei Steed", 66090, 46815, 1, 1, 0, "Horse", "Exaulted Argent Tournament"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66090 - 46815"] ={"Quel'dorei Steed", 66090, 46815, 1, 1, 0, "Horse", "Exaulted Argent Tournament"},</v>
       </c>
       <c r="O341" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38578,8 +38605,8 @@
         <v>66091 - 46816</v>
       </c>
       <c r="N342" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66091 - 46816"] +{"Sunreaver Hawkstrider", 66091, 46816, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66091 - 46816"] ={"Sunreaver Hawkstrider", 66091, 46816, 1, 1, 0, "Hawkstrider", "Champion's Seals"},</v>
       </c>
       <c r="O342" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38625,8 +38652,8 @@
         <v>66122 - 46778</v>
       </c>
       <c r="N343" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66122 - 46778"] +{"Magic Rooster", 66122, 46778, 1, 1, 0, "Rooster", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66122 - 46778"] ={"Magic Rooster", 66122, 46778, 1, 1, 0, "Rooster", "Duplicate"},</v>
       </c>
       <c r="O343" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38672,8 +38699,8 @@
         <v>66123 - 49290</v>
       </c>
       <c r="N344" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66123 - 49290"] +{"Magic Rooster", 66123, 49290, 1, 1, 0, "Rooster", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66123 - 49290"] ={"Magic Rooster", 66123, 49290, 1, 1, 0, "Rooster", "Duplicate"},</v>
       </c>
       <c r="O344" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38719,8 +38746,8 @@
         <v>66124 - 198631</v>
       </c>
       <c r="N345" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66124 - 198631"] +{"Magic Rooster", 66124, 198631, 1, 1, 0, "Rooster", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66124 - 198631"] ={"Magic Rooster", 66124, 198631, 1, 1, 0, "Rooster", "TCG"},</v>
       </c>
       <c r="O345" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38763,8 +38790,8 @@
         <v>66846 - 47101</v>
       </c>
       <c r="N346" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66846 - 47101"] +{"Ochre Skeletal Warhorse", 66846, 47101, 1, 1, 0, "DeadHorse", "Gold"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66846 - 47101"] ={"Ochre Skeletal Warhorse", 66846, 47101, 1, 1, 0, "DeadHorse", "Gold"},</v>
       </c>
       <c r="O346" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38810,8 +38837,8 @@
         <v>66847 - 47100</v>
       </c>
       <c r="N347" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66847 - 47100"] +{"Striped Dawnsaber", 66847, 47100, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66847 - 47100"] ={"Striped Dawnsaber", 66847, 47100, 0.6, 0.6, 0, "Saber", "Exaulted Darnasses"},</v>
       </c>
       <c r="O347" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38860,8 +38887,8 @@
         <v>66906 - 47179</v>
       </c>
       <c r="N348" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66906 - 47179"] +{"Argent Charger", 66906, 47179, 1, 1, 0, "Horse", "Daily"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66906 - 47179"] ={"Argent Charger", 66906, 47179, 1, 1, 0, "Horse", "Daily"},</v>
       </c>
       <c r="O348" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38907,8 +38934,8 @@
         <v>66907 - 0</v>
       </c>
       <c r="N349" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["66907 - 0"] +{"Argent Warhorse", 66907, 0, 0.6, 0.6, 0, "Horse", "Removed"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["66907 - 0"] ={"Argent Warhorse", 66907, 0, 0.6, 0.6, 0, "Horse", "Removed"},</v>
       </c>
       <c r="O349" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -38954,8 +38981,8 @@
         <v>67336 - 47840</v>
       </c>
       <c r="N350" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["67336 - 47840"] +{"Relentless Gladiator's Frost Wyrm", 67336, 47840, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["67336 - 47840"] ={"Relentless Gladiator's Frost Wyrm", 67336, 47840, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
       </c>
       <c r="O350" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39004,8 +39031,8 @@
         <v>67466 - 47180</v>
       </c>
       <c r="N351" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["67466 - 47180"] +{"Argent Warhorse", 67466, 47180, 1, 1, 0, "Horse", "Exaulted Argent Champion"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["67466 - 47180"] ={"Argent Warhorse", 67466, 47180, 1, 1, 0, "Horse", "Exaulted Argent Champion"},</v>
       </c>
       <c r="O351" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39048,8 +39075,8 @@
         <v>68056 - 49046</v>
       </c>
       <c r="N352" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["68056 - 49046"] +{"Swift Horde Wolf", 68056, 49046, 1, 1, 0, "Wolf", "Drop Trial of the Champion"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["68056 - 49046"] ={"Swift Horde Wolf", 68056, 49046, 1, 1, 0, "Wolf", "Drop Trial of the Champion"},</v>
       </c>
       <c r="O352" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39095,8 +39122,8 @@
         <v>68057 - 49044</v>
       </c>
       <c r="N353" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["68057 - 49044"] +{"Swift Alliance Steed", 68057, 49044, 1, 1, 0, "Horse", "Champion's Seals"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["68057 - 49044"] ={"Swift Alliance Steed", 68057, 49044, 1, 1, 0, "Horse", "Champion's Seals"},</v>
       </c>
       <c r="O353" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39142,8 +39169,8 @@
         <v>68187 - 49096</v>
       </c>
       <c r="N354" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["68187 - 49096"] +{"Crusader's White Warhorse", 68187, 49096, 1, 1, 0, "Horse", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["68187 - 49096"] ={"Crusader's White Warhorse", 68187, 49096, 1, 1, 0, "Horse", "Achievment"},</v>
       </c>
       <c r="O354" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39186,8 +39213,8 @@
         <v>68188 - 49098</v>
       </c>
       <c r="N355" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["68188 - 49098"] +{"Crusader's Black Warhorse", 68188, 49098, 1, 1, 0, "Horse", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["68188 - 49098"] ={"Crusader's Black Warhorse", 68188, 49098, 1, 1, 0, "Horse", "Achievment"},</v>
       </c>
       <c r="O355" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39236,8 +39263,8 @@
         <v>69395 - 49636</v>
       </c>
       <c r="N356" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["69395 - 49636"] +{"Onyxian Drake", 69395, 49636, 3.1, 3.1, 0, "Drake", "Drop Onyxia'a Lair"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["69395 - 49636"] ={"Onyxian Drake", 69395, 49636, 3.1, 3.1, 0, "Drake", "Drop Onyxia'a Lair"},</v>
       </c>
       <c r="O356" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39286,8 +39313,8 @@
         <v>71342 - 50250</v>
       </c>
       <c r="N357" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["71342 - 50250"] +{"X-45 Heartbreaker", 71342, 50250, 2.8, 0.6, 0, "Rocket", "Drop Valentines"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["71342 - 50250"] ={"X-45 Heartbreaker", 71342, 50250, 2.8, 0.6, 0, "Rocket", "Drop Valentines"},</v>
       </c>
       <c r="O357" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39333,8 +39360,8 @@
         <v>71810 - 50435</v>
       </c>
       <c r="N358" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["71810 - 50435"] +{"Wrathful Gladiator's Frost Wyrm", 71810, 50435, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["71810 - 50435"] ={"Wrathful Gladiator's Frost Wyrm", 71810, 50435, 3.1, 3.1, 0, "Wyrm", "Gladiator"},</v>
       </c>
       <c r="O358" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39383,8 +39410,8 @@
         <v>72286 - 50818</v>
       </c>
       <c r="N359" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["72286 - 50818"] +{"Invincible", 72286, 50818, 2.8, 2.8, 0, "Wyrm", "Drop Icecrown"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["72286 - 50818"] ={"Invincible", 72286, 50818, 2.8, 2.8, 0, "Wyrm", "Drop Icecrown"},</v>
       </c>
       <c r="O359" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39433,8 +39460,8 @@
         <v>72807 - 51955</v>
       </c>
       <c r="N360" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["72807 - 51955"] +{"Icebound Frostbrood Vanquisher", 72807, 51955, 3.1, 3.1, 0, "Wyrm", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["72807 - 51955"] ={"Icebound Frostbrood Vanquisher", 72807, 51955, 3.1, 3.1, 0, "Wyrm", "Achievment"},</v>
       </c>
       <c r="O360" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39483,8 +39510,8 @@
         <v>72808 - 51954</v>
       </c>
       <c r="N361" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["72808 - 51954"] +{"Bloodbathed Frostbrood Vanquisher", 72808, 51954, 3.1, 3.1, 0, "Wyrm", "Achievment"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["72808 - 51954"] ={"Bloodbathed Frostbrood Vanquisher", 72808, 51954, 3.1, 3.1, 0, "Wyrm", "Achievment"},</v>
       </c>
       <c r="O361" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39530,8 +39557,8 @@
         <v>73313 - 52200</v>
       </c>
       <c r="N362" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["73313 - 52200"] +{"Crimson Deathcharger", 73313, 52200, 1, 1, 0, "DeadHorse", "Shadowmourn Quest"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["73313 - 52200"] ={"Crimson Deathcharger", 73313, 52200, 1, 1, 0, "DeadHorse", "Shadowmourn Quest"},</v>
       </c>
       <c r="O362" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39577,8 +39604,8 @@
         <v>74856 - 54069</v>
       </c>
       <c r="N363" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["74856 - 54069"] +{"Blazing Hippogryph", 74856, 54069, 2.8, 2.8, 0, "Hippogryph", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["74856 - 54069"] ={"Blazing Hippogryph", 74856, 54069, 2.8, 2.8, 0, "Hippogryph", "TCG"},</v>
       </c>
       <c r="O363" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39624,8 +39651,8 @@
         <v>74918 - 54068</v>
       </c>
       <c r="N364" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["74918 - 54068"] +{"Wooly White Rhino", 74918, 54068, 1, 1, 0, "Rhino", "Duplicate"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["74918 - 54068"] ={"Wooly White Rhino", 74918, 54068, 1, 1, 0, "Rhino", "Duplicate"},</v>
       </c>
       <c r="O364" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39671,8 +39698,8 @@
         <v>75596 - 54797</v>
       </c>
       <c r="N365" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["75596 - 54797"] +{"Frosty Flying Carpet", 75596, 54797, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["75596 - 54797"] ={"Frosty Flying Carpet", 75596, 54797, 2.8, 2.8, 0, "Carpet", "Tailoring"},</v>
       </c>
       <c r="O365" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39718,8 +39745,8 @@
         <v>75614 - 54811</v>
       </c>
       <c r="N366" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["75614 - 54811"] +{"Celestial Steed", 75614, 54811, 2.8, 2.8, 0, "Horse", "Store"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["75614 - 54811"] ={"Celestial Steed", 75614, 54811, 2.8, 2.8, 0, "Horse", "Store"},</v>
       </c>
       <c r="O366" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39765,8 +39792,8 @@
         <v>75973 - 54860</v>
       </c>
       <c r="N367" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["75973 - 54860"] +{"X-53 Touring Rocket", 75973, 54860, 2.8, 2.8, 0, "Rocket", "Recruit a Friend"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["75973 - 54860"] ={"X-53 Touring Rocket", 75973, 54860, 2.8, 2.8, 0, "Rocket", "Recruit a Friend"},</v>
       </c>
       <c r="O367" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39812,8 +39839,8 @@
         <v>348459 - 184865</v>
       </c>
       <c r="N368" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["348459 - 184865"] +{"Reawakened Phase-Hunter", 348459, 184865, 1, 1, 0, "Warp Stalker", "Store"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["348459 - 184865"] ={"Reawakened Phase-Hunter", 348459, 184865, 1, 1, 0, "Warp Stalker", "Store"},</v>
       </c>
       <c r="O368" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39859,8 +39886,8 @@
         <v>387320 - 198630</v>
       </c>
       <c r="N369" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["387320 - 198630"] +{"Blazing Hippogryph", 387320, 198630, 1.5, 1.5, 0, "Hippogryph", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["387320 - 198630"] ={"Blazing Hippogryph", 387320, 198630, 1.5, 1.5, 0, "Hippogryph", "TCG"},</v>
       </c>
       <c r="O369" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
@@ -39906,23 +39933,70 @@
         <v>387321 - 198633</v>
       </c>
       <c r="N370" s="2" t="str">
-        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] +{""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
-        <v>["387321 - 198633"] +{"Wooly White Rhino", 387321, 198633, 1, 1, 0, "Rhino", "TCG"},</v>
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["387321 - 198633"] ={"Wooly White Rhino", 387321, 198633, 1, 1, 0, "Rhino", "TCG"},</v>
       </c>
       <c r="O370" s="2" t="str">
         <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
         <v>https://www.wowhead.com/wotlk/item=198633</v>
       </c>
     </row>
+    <row r="371" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A371">
+        <v>372677</v>
+      </c>
+      <c r="B371" t="s">
+        <v>760</v>
+      </c>
+      <c r="C371" t="s">
+        <v>761</v>
+      </c>
+      <c r="D371">
+        <v>2.8</v>
+      </c>
+      <c r="E371" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F371">
+        <v>0</v>
+      </c>
+      <c r="G371">
+        <v>192455</v>
+      </c>
+      <c r="H371" t="s">
+        <v>702</v>
+      </c>
+      <c r="I371">
+        <v>1</v>
+      </c>
+      <c r="J371">
+        <v>1</v>
+      </c>
+      <c r="L371">
+        <v>1</v>
+      </c>
+      <c r="M371" s="2" t="str">
+        <f>CONCATENATE(Table3[[#This Row],[Spell ID]]," - ",Table3[[#This Row],[ItemID]])</f>
+        <v>372677 - 192455</v>
+      </c>
+      <c r="N371" s="2" t="str">
+        <f>CONCATENATE("[""",Table3[[#This Row],[MountKey]],"""] ={""",Table3[[#This Row],[Name]],""", ",Table3[[#This Row],[Spell ID]],", ",Table3[[#This Row],[ItemID]],", ",Table3[[#This Row],[Speed]],", ",Table3[[#This Row],[MinSpeed]],", ",Table3[[#This Row],[SwimSpeed]],", """,Table3[[#This Row],[Category]],""", """,Table3[[#This Row],[Source]],"""},")</f>
+        <v>["372677 - 192455"] ={"Kalu'ak Whalebone Glider", 372677, 192455, 2.8, 0.6, 0, "Glider", "Store"},</v>
+      </c>
+      <c r="O371" s="2" t="str">
+        <f>CONCATENATE("https://www.wowhead.com/wotlk/item=",Table3[[#This Row],[ItemID]])</f>
+        <v>https://www.wowhead.com/wotlk/item=192455</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E371:E1048576 G1:G370">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="E371:E1048576 G1:G371">
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M370">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+  <conditionalFormatting sqref="M2:M371">
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>